<commit_message>
add function to check equation applicability. update tests.
</commit_message>
<xml_diff>
--- a/tests/mobile_network/path_loss_calc_validation.xlsx
+++ b/tests/mobile_network/path_loss_calc_validation.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1C01311C-F411-41E9-8D84-CF8B2E99A4F4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A87B0455-35FF-4BA3-B768-C3BA32731AC1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="21">
   <si>
     <t>urban</t>
   </si>
@@ -41,13 +41,55 @@
   </si>
   <si>
     <t>rural</t>
+  </si>
+  <si>
+    <t>PL1</t>
+  </si>
+  <si>
+    <t>PL2</t>
+  </si>
+  <si>
+    <t>settlement</t>
+  </si>
+  <si>
+    <t>ant_type</t>
+  </si>
+  <si>
+    <t>sight_type</t>
+  </si>
+  <si>
+    <t>freq (Hz)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>breakpoint (d'BP)</t>
+  </si>
+  <si>
+    <t>breakpoint (dBP)</t>
+  </si>
+  <si>
+    <t>building_height (h)</t>
+  </si>
+  <si>
+    <t>street_width (w)</t>
+  </si>
+  <si>
+    <t>distance (d)</t>
+  </si>
+  <si>
+    <t>ant_height (hBS)</t>
+  </si>
+  <si>
+    <t>UE_height (hUT)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,13 +97,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -76,9 +149,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -359,132 +445,545 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D9"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="A9:D9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K7" sqref="A7:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" customWidth="1"/>
+    <col min="11" max="11" width="10" customWidth="1"/>
+    <col min="12" max="12" width="6.7109375" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <f>4*G2*M2*E2/(300000000)</f>
+        <v>700</v>
+      </c>
+      <c r="C2" s="3">
+        <f>22*LOG10(F2)+28+20*LOG10(E2/1000000000)</f>
+        <v>98.258700982397926</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="2">
+        <v>3500000000</v>
+      </c>
+      <c r="F2" s="2">
+        <v>500</v>
+      </c>
+      <c r="G2" s="2">
+        <v>10</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="L2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <f>4*G3*M3*E3/(300000000)</f>
+        <v>700</v>
+      </c>
+      <c r="C3" s="3">
+        <f>40*LOG10(F3)+7.8-18*LOG10(G3)-18*LOG10(M3)+2*LOG10(E3/1000000000)</f>
+        <v>107.71849342569828</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="2">
+        <v>3500000000</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1000</v>
+      </c>
+      <c r="G3" s="2">
+        <v>10</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="I3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1">
-        <f>40*LOG10(1000)+7.8-18*LOG10(10)-18*LOG10(1.5)+2*LOG10(3.5)</f>
-        <v>107.71849342569828</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="M3" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="3">
+        <f>(36.7*LOG10(F4)+22.7+26*LOG10(E4/1000000000))</f>
+        <v>135.89796831223907</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="2">
+        <v>3500000000</v>
+      </c>
+      <c r="F4" s="2">
+        <v>500</v>
+      </c>
+      <c r="G4" s="2">
+        <v>10</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="L4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1">
-        <f>(36.7*LOG10(1000)+22.7+26*LOG10(3.5))</f>
-        <v>146.94576915310716</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="M4" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <f>4*G5*M5*E5/(300000000)</f>
+        <v>1750</v>
+      </c>
+      <c r="C5" s="9">
+        <f>22*LOG10(F5)+28+20*LOG10(E5/1000000000)</f>
+        <v>98.258700982397926</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="8">
+        <v>3500000000</v>
+      </c>
+      <c r="F5" s="8">
+        <v>500</v>
+      </c>
+      <c r="G5" s="8">
+        <v>25</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="8">
+        <v>20</v>
+      </c>
+      <c r="J5" s="8">
+        <v>20</v>
+      </c>
+      <c r="K5" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B4" t="s">
+      <c r="L5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="8">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <f>4*G6*M6*E6/(300000000)</f>
+        <v>1750</v>
+      </c>
+      <c r="C6" s="9">
+        <f>40*LOG10(F6)+7.8-18*LOG10(G6)-18*LOG10(M6)+2*LOG10(E6/1000000000)</f>
+        <v>112.59677309616087</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="8">
+        <v>3500000000</v>
+      </c>
+      <c r="F6" s="8">
+        <v>2000</v>
+      </c>
+      <c r="G6" s="8">
+        <v>25</v>
+      </c>
+      <c r="H6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="I6" s="8">
+        <v>20</v>
+      </c>
+      <c r="J6" s="8">
+        <v>20</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="L6" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="1">
-        <f>40*LOG10(1000)+7.8-18*LOG10(25)-18*LOG10(1.5)+2*LOG10(3.5)</f>
-        <v>100.55557326960161</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="M6" s="8">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <f>4*G7*M7*E7/(300000000)</f>
+        <v>1750</v>
+      </c>
+      <c r="C7" s="9">
+        <f>161.04-7.1*LOG(J7)+7.5*LOG10(I7)-(24.37-3.7*(I7/G7)^2)*LOG10(G7)+(43.42-3.1*LOG10(G7))*(LOG10(F7)-3)+20*LOG10(E7/1000000000)-(3.2*(LOG10(11.75*M7))^2-4.97)</f>
+        <v>141.68521586142342</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="8">
+        <v>3500000000</v>
+      </c>
+      <c r="F7" s="8">
+        <v>1000</v>
+      </c>
+      <c r="G7" s="8">
+        <v>25</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="8">
+        <v>20</v>
+      </c>
+      <c r="J7" s="8">
+        <v>20</v>
+      </c>
+      <c r="K7" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B5" t="s">
+      <c r="L7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="M7" s="8">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <f>4*G8*M8*E8/(300000000)</f>
+        <v>2450</v>
+      </c>
+      <c r="B8" s="7">
+        <f>2*PI()*G8*M8*E8/(300000000)</f>
+        <v>3848.4510006474966</v>
+      </c>
+      <c r="C8" s="7">
+        <f>20*LOG10(40*PI()*F8*(E8/1000000000)/3)+MIN(0.03*I8^1.72, 10)*LOG10(F8)-MIN(0.044*I8^1.72,14.77)+0.002*LOG10(I8)*F8</f>
+        <v>107.73724739020315</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="6">
+        <v>3500000000</v>
+      </c>
+      <c r="F8" s="6">
+        <v>1000</v>
+      </c>
+      <c r="G8" s="6">
+        <v>35</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="I8" s="6">
+        <v>10</v>
+      </c>
+      <c r="J8" s="6">
+        <v>20</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M8" s="6">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <f>4*G9*M9*E9/(300000000)</f>
+        <v>2450</v>
+      </c>
+      <c r="B9" s="7">
+        <f>2*PI()*G9*M9*E9/(300000000)</f>
+        <v>3848.4510006474966</v>
+      </c>
+      <c r="C9" s="7">
+        <f xml:space="preserve"> (20*LOG10(40*PI()*B9*(E9/1000000000)/3)+MIN(0.03*I9^1.72, 10)*LOG10(B9)-MIN(0.044*I9^1.72,14.77)+0.002*LOG10(I9)*B9)</f>
+        <v>126.06135593614999</v>
+      </c>
+      <c r="D9" s="7">
+        <f xml:space="preserve"> C9+40*LOG10(F9/B9)</f>
+        <v>126.73231713348109</v>
+      </c>
+      <c r="E9" s="6">
+        <v>3500000000</v>
+      </c>
+      <c r="F9" s="6">
+        <v>4000</v>
+      </c>
+      <c r="G9" s="6">
+        <v>35</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="6">
+        <v>10</v>
+      </c>
+      <c r="J9" s="6">
+        <v>20</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M9" s="6">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <f>4*G10*M10*E10/(300000000)</f>
+        <v>2450</v>
+      </c>
+      <c r="C10" s="7">
+        <f>161.04-7.1*LOG10(J10)+7.5*LOG10(I10)-(24.37-3.7*(I10/G10)^2)*LOG10(G10)+(43.42-3.1*LOG10(G10))*(LOG10(F10)-3)+20*LOG10(E10/1000000000)-(3.2*(LOG10(11.75*M10))^2-4.97)</f>
+        <v>121.39259135453526</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="6">
+        <v>3500000000</v>
+      </c>
+      <c r="F10" s="6">
+        <v>500</v>
+      </c>
+      <c r="G10" s="6">
+        <v>35</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="6">
+        <v>10</v>
+      </c>
+      <c r="J10" s="6">
+        <v>20</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L10" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="1">
-        <f>161.04-7.1*LOG(20)+7.5*LOG10(20)-(24.37-3.7*(20/25)^2)*LOG10(25)+(43.42-3.1*LOG10(25))*(LOG10(1000)-3)+20*LOG10(3.5)-(3.2*(LOG10(11.75*1.5))^2-4.97)</f>
-        <v>141.68521586142342</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="M10" s="6">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <f>4*G11*M11*E11/(300000000)</f>
+        <v>2450</v>
+      </c>
+      <c r="B11" s="5">
+        <f>2*PI()*G11*M11*E11/(300000000)</f>
+        <v>3848.4510006474966</v>
+      </c>
+      <c r="C11" s="5">
+        <f>20*LOG10(40*PI()*F11*(E11/1000000000)/3)+MIN(0.03*I11^1.72, 10)*LOG10(F11)-MIN(0.044*I11^1.72,14.77)+0.002*LOG10(I11)*F11</f>
+        <v>107.73724739020315</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="4">
+        <v>3500000000</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1000</v>
+      </c>
+      <c r="G11" s="4">
+        <v>35</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
+      <c r="I11" s="4">
+        <v>10</v>
+      </c>
+      <c r="J11" s="4">
+        <v>20</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D6" t="e">
-        <f>20*LOG10(40*PI*1000*3.5/3)+MIN(0.03*25^1.72, 10)*LOG10(1000)-MIN(0.044*25^1.72,14.77)+0.002*LOG10(25)*1000</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="M11" s="4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <f>4*G12*M12*E12/(300000000)</f>
+        <v>2450</v>
+      </c>
+      <c r="B12" s="5">
+        <f>2*PI()*G12*M12*E12/(300000000)</f>
+        <v>3848.4510006474966</v>
+      </c>
+      <c r="C12" s="5">
+        <f xml:space="preserve"> (20*LOG10(40*PI()*B12*(E12/1000000000)/3)+MIN(0.03*I12^1.72, 10)*LOG10(B12)-MIN(0.044*I12^1.72,14.77)+0.002*LOG10(I12)*B12)</f>
+        <v>126.06135593614999</v>
+      </c>
+      <c r="D12" s="5">
+        <f xml:space="preserve"> C12+40*LOG10(F12/B12)</f>
+        <v>126.73231713348109</v>
+      </c>
+      <c r="E12" s="4">
+        <v>3500000000</v>
+      </c>
+      <c r="F12" s="4">
+        <v>4000</v>
+      </c>
+      <c r="G12" s="4">
+        <v>35</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
+      <c r="I12" s="4">
+        <v>10</v>
+      </c>
+      <c r="J12" s="4">
+        <v>20</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="M12" s="4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <f>4*G13*M13*E13/(300000000)</f>
+        <v>2450</v>
+      </c>
+      <c r="C13" s="5">
+        <f>161.04-7.1*LOG10(J13)+7.5*LOG10(I13)-(24.37-3.7*(I13/G13)^2)*LOG10(G13)+(43.42-3.1*LOG10(G13))*(LOG10(F13)-3)+20*LOG10(E13/1000000000)-(3.2*(LOG10(11.75*M13))^2-4.97)</f>
+        <v>121.39259135453526</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="4">
+        <v>3500000000</v>
+      </c>
+      <c r="F13" s="4">
+        <v>500</v>
+      </c>
+      <c r="G13" s="4">
+        <v>35</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="4">
+        <v>10</v>
+      </c>
+      <c r="J13" s="4">
+        <v>20</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="1">
-        <f>161.04-7.1*LOG10(20)+7.5*LOG10(20)-(24.37-3.7*(20/25)^2)*LOG10(25)+(43.42-3.1*LOG10(25))*(LOG10(1000)-3)+20*LOG10(3.5)-(3.2*(LOG10(11.75*1.5))^2-4.97)</f>
-        <v>141.68521586142342</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" t="e">
-        <f>20*LOG10(40*PI*1000*3.5/3)+MIN(0.03*20^1.72, 10)*LOG10(1000)-MIN(0.044*20^1.72,14.77)+0.002*LOG10(20)*1000</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="1">
-        <f>161.04-7.1*LOG10(20)+7.5*LOG10(20)-(24.37-3.7*(20/25)^2)*LOG10(25)+(43.42-3.1*LOG10(25))*(LOG10(1000)-3)+20*LOG10(3.5)-(3.2*(LOG10(11.75*1.5))^2-4.97)</f>
-        <v>141.68521586142342</v>
+      <c r="M13" s="4">
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Major changes to simulator
</commit_message>
<xml_diff>
--- a/tests/mobile_network/path_loss_calc_validation.xlsx
+++ b/tests/mobile_network/path_loss_calc_validation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\digital_comms\tests\mobile_network\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CED7E15-71E2-44FE-83BC-320CC26B802C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA55877-BA49-4F88-9C54-957B425AE651}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="48">
   <si>
     <t>Free space path loss model</t>
   </si>
@@ -162,6 +162,18 @@
   </si>
   <si>
     <t>Extended Hata</t>
+  </si>
+  <si>
+    <t>uMA NLOS Optional model</t>
+  </si>
+  <si>
+    <t>3D Distance (m)</t>
+  </si>
+  <si>
+    <t>2D Distance (m)</t>
+  </si>
+  <si>
+    <t>Frequency (GHz)</t>
   </si>
 </sst>
 </file>
@@ -332,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -355,7 +367,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="15"/>
     </xf>
@@ -507,6 +518,18 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -824,8 +847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O40" sqref="O40"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3:S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -847,7 +870,7 @@
     <col min="15" max="15" width="8.5703125" customWidth="1"/>
     <col min="16" max="16" width="9.28515625" customWidth="1"/>
     <col min="17" max="17" width="14.5703125" customWidth="1"/>
-    <col min="18" max="18" width="14.5703125" style="24" customWidth="1"/>
+    <col min="18" max="18" width="14.5703125" style="23" customWidth="1"/>
     <col min="19" max="19" width="12.42578125" customWidth="1"/>
     <col min="20" max="20" width="12.85546875" customWidth="1"/>
     <col min="21" max="21" width="14.7109375" customWidth="1"/>
@@ -856,17 +879,24 @@
     <col min="24" max="1026" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="70" t="s">
+    <row r="1" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-    </row>
-    <row r="3" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="N2" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="O2" s="68"/>
+      <c r="P2" s="68"/>
+      <c r="Q2" s="68"/>
+      <c r="R2" s="68"/>
+    </row>
+    <row r="3" spans="1:19" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -895,9 +925,24 @@
       <c r="K3" s="3"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="P3" s="70" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="S3" s="3"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>800</v>
       </c>
@@ -930,9 +975,28 @@
         <f t="shared" ref="K4:K18" si="1">32.4+10*LOG10(POWER(((I4-J4)/1000),2)+POWER(H4,2))+20*LOG10(G4)</f>
         <v>84.455287181739891</v>
       </c>
-      <c r="N4" s="8"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N4" s="5">
+        <v>3.5</v>
+      </c>
+      <c r="O4" s="6">
+        <v>1000</v>
+      </c>
+      <c r="P4" s="37">
+        <f>SQRT(POWER(O4,2)+POWER((Q4-R4),2))</f>
+        <v>1000.4060425647178</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>30</v>
+      </c>
+      <c r="R4" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="S4" s="7">
+        <f>32.4+20*LOG10(N4)+30*LOG10(P4)</f>
+        <v>133.28665007461876</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>800</v>
       </c>
@@ -965,9 +1029,28 @@
         <f t="shared" si="1"/>
         <v>96.483281452823618</v>
       </c>
-      <c r="N5" s="8"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N5" s="5">
+        <v>3.5</v>
+      </c>
+      <c r="O5" s="6">
+        <v>5000</v>
+      </c>
+      <c r="P5" s="37">
+        <f>SQRT(POWER(O5,2)+POWER((Q5-R5),2))</f>
+        <v>5000.0812243402606</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>30</v>
+      </c>
+      <c r="R5" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="S5" s="7">
+        <f>32.4+20*LOG10(N5)+30*LOG10(P5)</f>
+        <v>154.25067266706358</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>800</v>
       </c>
@@ -1000,9 +1083,28 @@
         <f t="shared" si="1"/>
         <v>100.00461676731632</v>
       </c>
-      <c r="N6" s="8"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N6" s="5">
+        <v>3.5</v>
+      </c>
+      <c r="O6" s="6">
+        <v>10000</v>
+      </c>
+      <c r="P6" s="37">
+        <f>SQRT(POWER(O6,2)+POWER((Q6-R6),2))</f>
+        <v>10000.040612417532</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>30</v>
+      </c>
+      <c r="R6" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="S6" s="7">
+        <f>32.4+20*LOG10(N6)+30*LOG10(P6)</f>
+        <v>163.28141380014455</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>800</v>
       </c>
@@ -1035,9 +1137,28 @@
         <f t="shared" si="1"/>
         <v>102.50322003311018</v>
       </c>
-      <c r="N7" s="8"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N7" s="72">
+        <v>3.5</v>
+      </c>
+      <c r="O7" s="62">
+        <v>20000</v>
+      </c>
+      <c r="P7" s="44">
+        <f>SQRT(POWER(O7,2)+POWER((Q7-R7),2))</f>
+        <v>20000.02030623969</v>
+      </c>
+      <c r="Q7" s="62">
+        <v>30</v>
+      </c>
+      <c r="R7" s="62">
+        <v>1.5</v>
+      </c>
+      <c r="S7" s="12">
+        <f>32.4+20*LOG10(N7)+30*LOG10(P7)</f>
+        <v>172.31227398525002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>800</v>
       </c>
@@ -1070,9 +1191,14 @@
         <f>32.4+10*LOG10(POWER(((I8-J8)/1000),2)+POWER(H8,2))+20*LOG10(G8)</f>
         <v>104.44134092654426</v>
       </c>
-      <c r="N8" s="8"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N8" s="73"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="37"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="55"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>1800</v>
       </c>
@@ -1105,8 +1231,14 @@
         <f t="shared" si="1"/>
         <v>91.498937543967116</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N9" s="73"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="37"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="55"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>1800</v>
       </c>
@@ -1140,7 +1272,7 @@
         <v>103.52693181505086</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>1800</v>
       </c>
@@ -1174,7 +1306,7 @@
         <v>107.04826712954356</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>1800</v>
       </c>
@@ -1207,8 +1339,14 @@
         <f t="shared" si="1"/>
         <v>109.54687039533742</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="36"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="55"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>1800</v>
       </c>
@@ -1241,8 +1379,14 @@
         <f t="shared" si="1"/>
         <v>111.48499128877151</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="36"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="55"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>2600</v>
       </c>
@@ -1275,8 +1419,14 @@
         <f t="shared" si="1"/>
         <v>100.70299308449185</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="36"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="55"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>2600</v>
       </c>
@@ -1309,11 +1459,16 @@
         <f t="shared" si="1"/>
         <v>106.72094867240109</v>
       </c>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="36"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="55"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>2600</v>
       </c>
@@ -1346,7 +1501,13 @@
         <f t="shared" si="1"/>
         <v>110.2422839868938</v>
       </c>
-      <c r="L16" s="10"/>
+      <c r="L16" s="9"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="36"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="55"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
@@ -1381,67 +1542,79 @@
         <f t="shared" si="1"/>
         <v>112.74088725268766</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" s="14" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="11">
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="36"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="55"/>
+    </row>
+    <row r="18" spans="1:20" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="10">
         <v>2600</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18" s="11">
         <v>5</v>
       </c>
-      <c r="C18" s="12">
-        <v>20</v>
-      </c>
-      <c r="D18" s="12">
-        <v>1.5</v>
-      </c>
-      <c r="E18" s="13">
+      <c r="C18" s="11">
+        <v>20</v>
+      </c>
+      <c r="D18" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="E18" s="12">
         <f t="shared" si="0"/>
         <v>114.67892650064434</v>
       </c>
-      <c r="G18" s="11">
+      <c r="G18" s="10">
         <v>2600</v>
       </c>
-      <c r="H18" s="12">
+      <c r="H18" s="11">
         <v>5</v>
       </c>
-      <c r="I18" s="63">
+      <c r="I18" s="62">
         <v>30</v>
       </c>
-      <c r="J18" s="12">
-        <v>1.5</v>
-      </c>
-      <c r="K18" s="13">
+      <c r="J18" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="K18" s="12">
         <f t="shared" si="1"/>
         <v>114.67900814612173</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="55"/>
-      <c r="B19" s="55"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="56"/>
+      <c r="N18" s="54"/>
+      <c r="O18" s="54"/>
+      <c r="P18" s="71"/>
+      <c r="Q18" s="54"/>
+      <c r="R18" s="54"/>
+      <c r="S18" s="55"/>
+    </row>
+    <row r="19" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="54"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="55"/>
     </row>
     <row r="20" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="69" t="s">
+      <c r="A20" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="69"/>
-      <c r="C20" s="69"/>
-      <c r="D20" s="69"/>
-      <c r="E20" s="69"/>
-      <c r="F20" s="69"/>
-      <c r="G20" s="69"/>
-      <c r="H20" s="69"/>
-      <c r="I20" s="69"/>
-      <c r="J20" s="69"/>
-      <c r="K20" s="69"/>
-      <c r="L20" s="69"/>
-      <c r="M20" s="69"/>
-      <c r="N20" s="69"/>
-    </row>
-    <row r="21" spans="1:20" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B20" s="68"/>
+      <c r="C20" s="68"/>
+      <c r="D20" s="68"/>
+      <c r="E20" s="68"/>
+      <c r="F20" s="68"/>
+      <c r="G20" s="68"/>
+      <c r="H20" s="68"/>
+      <c r="I20" s="68"/>
+      <c r="J20" s="68"/>
+      <c r="K20" s="68"/>
+      <c r="L20" s="68"/>
+      <c r="M20" s="68"/>
+      <c r="N20" s="68"/>
+    </row>
+    <row r="21" spans="1:20" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
@@ -1481,7 +1654,7 @@
       <c r="M21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N21" s="15" t="s">
+      <c r="N21" s="14" t="s">
         <v>14</v>
       </c>
       <c r="P21" s="1" t="s">
@@ -1493,7 +1666,7 @@
       <c r="R21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="S21" s="49"/>
+      <c r="S21" s="48"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
@@ -1525,24 +1698,24 @@
         <f t="shared" ref="I22:I53" si="3">MAX(F22,G22)</f>
         <v>20</v>
       </c>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
       <c r="L22" s="6">
         <v>1</v>
       </c>
       <c r="M22" s="6"/>
-      <c r="N22" s="64">
+      <c r="N22" s="63">
         <f>32.4+(20*LOG($D$22))+(10*LOG(POWER($E$22,2)+POWER(($I$22-$H$22),2)/(POWER(10,6))))</f>
         <v>59.167301802519702</v>
       </c>
-      <c r="P22" s="50"/>
-      <c r="Q22" s="37"/>
-      <c r="R22" s="37"/>
-      <c r="S22" s="18">
+      <c r="P22" s="49"/>
+      <c r="Q22" s="36"/>
+      <c r="R22" s="36"/>
+      <c r="S22" s="17">
         <f>32.4+(20*LOG($D$22))+(10*LOG(POWER($E$22,2)+POWER(($I$22-$H$22),2)/(POWER(10,6))))</f>
         <v>59.167301802519702</v>
       </c>
-      <c r="T22" s="53"/>
+      <c r="T22" s="52"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
@@ -1574,11 +1747,11 @@
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J23" s="17">
+      <c r="J23" s="16">
         <f>(1.1*LOG($D23)-0.7)*MIN(10,$H23)-(1.56*LOG($D23)-0.8)+MAX(0,20*LOG($H23/10))</f>
         <v>-6.999999999999984E-2</v>
       </c>
-      <c r="K23" s="17">
+      <c r="K23" s="16">
         <f>MIN(0,20*LOG($I23/30))</f>
         <v>-3.5218251811136252</v>
       </c>
@@ -1586,24 +1759,24 @@
         <v>1</v>
       </c>
       <c r="M23" s="6"/>
-      <c r="N23" s="64">
+      <c r="N23" s="63">
         <f>69.6+26.2*LOG(150)-20*LOG(150/$D$23)-13.82*LOG(MAX(30,$I$23))+(44.9-6.55*LOG(MAX(30,$I$23)))*POWER((LOG($E$23)),$L$23)-$P$23-$Q$23</f>
         <v>81.648657648642157</v>
       </c>
-      <c r="P23" s="50">
+      <c r="P23" s="49">
         <f>(1.1*LOG($D23)-0.7)*MIN(10,$H23)-(1.56*LOG($D23)-0.8)+MAX(0,20*LOG($H23/10))</f>
         <v>-6.999999999999984E-2</v>
       </c>
-      <c r="Q23" s="17">
+      <c r="Q23" s="16">
         <f>MIN(0,20*LOG($I23/30))</f>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="R23" s="17"/>
-      <c r="S23" s="18">
+      <c r="R23" s="16"/>
+      <c r="S23" s="17">
         <f>69.6+26.2*LOG(150)-20*LOG(150/$D$23)-13.82*LOG(MAX(30,$I$23))+(44.9-6.55*LOG(MAX(30,$I$23)))*POWER((LOG($E$23)),$L$23)-$P$23-$Q$23</f>
         <v>81.648657648642157</v>
       </c>
-      <c r="T23" s="53"/>
+      <c r="T23" s="52"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
@@ -1635,11 +1808,11 @@
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J24" s="17">
+      <c r="J24" s="16">
         <f t="shared" ref="J24:J53" si="4">(1.1*LOG($D24)-0.7)*MIN(10,$H24)-(1.56*LOG($D24)-0.8)+MAX(0,20*LOG($H24/10))</f>
         <v>-6.999999999999984E-2</v>
       </c>
-      <c r="K24" s="17">
+      <c r="K24" s="16">
         <f t="shared" ref="K24:K53" si="5">MIN(0,20*LOG($I24/30))</f>
         <v>-3.5218251811136252</v>
       </c>
@@ -1647,24 +1820,24 @@
         <v>1</v>
       </c>
       <c r="M24" s="6"/>
-      <c r="N24" s="64">
+      <c r="N24" s="63">
         <f>69.6+26.2*LOG(150)-20*LOG(150/$D$24)-13.82*LOG(MAX(30,$I$24))+(44.9-6.55*LOG(MAX(30,$I$24)))*POWER((LOG($E$24)),$L$24)-$P$24-$Q$24</f>
         <v>81.648657648642157</v>
       </c>
-      <c r="P24" s="50">
+      <c r="P24" s="49">
         <f t="shared" ref="P24:P53" si="6">(1.1*LOG($D24)-0.7)*MIN(10,$H24)-(1.56*LOG($D24)-0.8)+MAX(0,20*LOG($H24/10))</f>
         <v>-6.999999999999984E-2</v>
       </c>
-      <c r="Q24" s="17">
+      <c r="Q24" s="16">
         <f t="shared" ref="Q24:Q53" si="7">MIN(0,20*LOG($I24/30))</f>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="R24" s="17"/>
-      <c r="S24" s="18">
+      <c r="R24" s="16"/>
+      <c r="S24" s="17">
         <f>69.6+26.2*LOG(150)-20*LOG(150/$D$24)-13.82*LOG(MAX(30,$I$24))+(44.9-6.55*LOG(MAX(30,$I$24)))*POWER((LOG($E$24)),$L$24)-$P$24-$Q$24</f>
         <v>81.648657648642157</v>
       </c>
-      <c r="T24" s="53"/>
+      <c r="T24" s="52"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
@@ -1696,11 +1869,11 @@
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J25" s="17">
+      <c r="J25" s="16">
         <f t="shared" si="4"/>
         <v>1.1278098829275329E-2</v>
       </c>
-      <c r="K25" s="17">
+      <c r="K25" s="16">
         <f t="shared" si="5"/>
         <v>-3.5218251811136252</v>
       </c>
@@ -1708,24 +1881,24 @@
         <v>1</v>
       </c>
       <c r="M25" s="6"/>
-      <c r="N25" s="64">
+      <c r="N25" s="63">
         <f>69.6+26.2*LOG($D$25)-13.82*LOG(MAX(30,$I$25))+(44.9-6.55*LOG(MAX(30,$I$25)))*POWER((LOG($E$25)),$L$25)-$P$25-$Q$25</f>
         <v>104.13657140285657</v>
       </c>
-      <c r="P25" s="50">
+      <c r="P25" s="49">
         <f t="shared" si="6"/>
         <v>1.1278098829275329E-2</v>
       </c>
-      <c r="Q25" s="17">
+      <c r="Q25" s="16">
         <f t="shared" si="7"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="R25" s="17"/>
-      <c r="S25" s="18">
+      <c r="R25" s="16"/>
+      <c r="S25" s="17">
         <f>69.6+26.2*LOG($D$25)-13.82*LOG(MAX(30,$I$25))+(44.9-6.55*LOG(MAX(30,$I$25)))*POWER((LOG($E$25)),$L$25)-$P$25-$Q$25</f>
         <v>104.13657140285657</v>
       </c>
-      <c r="T25" s="53"/>
+      <c r="T25" s="52"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
@@ -1757,11 +1930,11 @@
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J26" s="17">
+      <c r="J26" s="16">
         <f t="shared" si="4"/>
         <v>1.1278098829275329E-2</v>
       </c>
-      <c r="K26" s="17">
+      <c r="K26" s="16">
         <f t="shared" si="5"/>
         <v>-3.5218251811136252</v>
       </c>
@@ -1769,24 +1942,24 @@
         <v>1</v>
       </c>
       <c r="M26" s="6"/>
-      <c r="N26" s="64">
+      <c r="N26" s="63">
         <f>69.6+26.2*LOG($D$26)-13.82*LOG(MAX(30,$I$26))+(44.9-6.55*LOG(MAX(30,$I$26)))*POWER((LOG($E$26)),$L$26)-$P$26-$Q$26</f>
         <v>104.13657140285657</v>
       </c>
-      <c r="P26" s="50">
+      <c r="P26" s="49">
         <f t="shared" si="6"/>
         <v>1.1278098829275329E-2</v>
       </c>
-      <c r="Q26" s="17">
+      <c r="Q26" s="16">
         <f t="shared" si="7"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="R26" s="17"/>
-      <c r="S26" s="18">
+      <c r="R26" s="16"/>
+      <c r="S26" s="17">
         <f>69.6+26.2*LOG($D$26)-13.82*LOG(MAX(30,$I$26))+(44.9-6.55*LOG(MAX(30,$I$26)))*POWER((LOG($E$26)),$L$26)-$P$26-$Q$26</f>
         <v>104.13657140285657</v>
       </c>
-      <c r="T26" s="53"/>
+      <c r="T26" s="52"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
@@ -1818,11 +1991,11 @@
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J27" s="17">
+      <c r="J27" s="16">
         <f t="shared" si="4"/>
         <v>4.2974525459298363E-2</v>
       </c>
-      <c r="K27" s="17">
+      <c r="K27" s="16">
         <f t="shared" si="5"/>
         <v>-3.5218251811136252</v>
       </c>
@@ -1830,24 +2003,24 @@
         <v>1</v>
       </c>
       <c r="M27" s="6"/>
-      <c r="N27" s="64">
+      <c r="N27" s="63">
         <f>46.3+33.9*LOG($D$27)-13.82*LOG(MAX(30,$I$27))+(44.9-6.55*LOG(MAX(30,$I$27)))*POWER((LOG($E$27)),$L$27)-$P$27-$Q$27</f>
         <v>115.0976552400397</v>
       </c>
-      <c r="P27" s="50">
+      <c r="P27" s="49">
         <f t="shared" si="6"/>
         <v>4.2974525459298363E-2</v>
       </c>
-      <c r="Q27" s="17">
+      <c r="Q27" s="16">
         <f t="shared" si="7"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="R27" s="17"/>
-      <c r="S27" s="18">
+      <c r="R27" s="16"/>
+      <c r="S27" s="17">
         <f>46.3+33.9*LOG($D$27)-13.82*LOG(MAX(30,$I$27))+(44.9-6.55*LOG(MAX(30,$I$27)))*POWER((LOG($E$27)),$L$27)-$P$27-$Q$27</f>
         <v>115.0976552400397</v>
       </c>
-      <c r="T27" s="53"/>
+      <c r="T27" s="52"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
@@ -1879,11 +2052,11 @@
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J28" s="17">
+      <c r="J28" s="16">
         <f t="shared" si="4"/>
         <v>4.2974525459298363E-2</v>
       </c>
-      <c r="K28" s="17">
+      <c r="K28" s="16">
         <f t="shared" si="5"/>
         <v>-3.5218251811136252</v>
       </c>
@@ -1891,24 +2064,24 @@
         <v>1</v>
       </c>
       <c r="M28" s="6"/>
-      <c r="N28" s="64">
+      <c r="N28" s="63">
         <f>46.3+33.9*LOG($D$28)-13.82*LOG(MAX(30,$I$28))+(44.9-6.55*LOG(MAX(30,$I$28)))*POWER((LOG($E$28)),$L$28)-$P$28-$Q$28</f>
         <v>115.0976552400397</v>
       </c>
-      <c r="P28" s="50">
+      <c r="P28" s="49">
         <f t="shared" si="6"/>
         <v>4.2974525459298363E-2</v>
       </c>
-      <c r="Q28" s="17">
+      <c r="Q28" s="16">
         <f t="shared" si="7"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="R28" s="17"/>
-      <c r="S28" s="18">
+      <c r="R28" s="16"/>
+      <c r="S28" s="17">
         <f>46.3+33.9*LOG($D$28)-13.82*LOG(MAX(30,$I$28))+(44.9-6.55*LOG(MAX(30,$I$28)))*POWER((LOG($E$28)),$L$28)-$P$28-$Q$28</f>
         <v>115.0976552400397</v>
       </c>
-      <c r="T28" s="53"/>
+      <c r="T28" s="52"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
@@ -1940,36 +2113,36 @@
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J29" s="17">
+      <c r="J29" s="16">
         <f t="shared" si="4"/>
         <v>4.8999736526052828E-2</v>
       </c>
-      <c r="K29" s="17">
+      <c r="K29" s="16">
         <f t="shared" si="5"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="L29" s="19">
+      <c r="L29" s="18">
         <v>1</v>
       </c>
       <c r="M29" s="6"/>
-      <c r="N29" s="64">
+      <c r="N29" s="63">
         <f>46.3+33.9*LOG(2000)+10*LOG($D$29/2000)-13.82*LOG(MAX(30,$I$29))+(44.9-6.55*LOG(MAX(30,$I$29)))*POWER((LOG($E$29)),$L$29)-$P$29-$Q$29</f>
         <v>116.85470194967921</v>
       </c>
-      <c r="P29" s="50">
+      <c r="P29" s="49">
         <f t="shared" si="6"/>
         <v>4.8999736526052828E-2</v>
       </c>
-      <c r="Q29" s="17">
+      <c r="Q29" s="16">
         <f t="shared" si="7"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="R29" s="17"/>
-      <c r="S29" s="18">
+      <c r="R29" s="16"/>
+      <c r="S29" s="17">
         <f>46.3+33.9*LOG(2000)+10*LOG($D$29/2000)-13.82*LOG(MAX(30,$I$29))+(44.9-6.55*LOG(MAX(30,$I$29)))*POWER((LOG($E$29)),$L$29)-$P$29-$Q$29</f>
         <v>116.85470194967921</v>
       </c>
-      <c r="T29" s="53"/>
+      <c r="T29" s="52"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
@@ -2001,11 +2174,11 @@
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J30" s="17">
+      <c r="J30" s="16">
         <f t="shared" si="4"/>
         <v>4.8999736526052828E-2</v>
       </c>
-      <c r="K30" s="17">
+      <c r="K30" s="16">
         <f t="shared" si="5"/>
         <v>-3.5218251811136252</v>
       </c>
@@ -2013,24 +2186,24 @@
         <v>1</v>
       </c>
       <c r="M30" s="6"/>
-      <c r="N30" s="64">
+      <c r="N30" s="63">
         <f>46.3+33.9*LOG(2000)+10*LOG($D$30/2000)-13.82*LOG(MAX(30,$I$30))+(44.9-6.55*LOG(MAX(30,$I$30)))*POWER((LOG($E$30)),$L$30)-$P$30-$Q$30</f>
         <v>116.85470194967921</v>
       </c>
-      <c r="P30" s="50">
+      <c r="P30" s="49">
         <f t="shared" si="6"/>
         <v>4.8999736526052828E-2</v>
       </c>
-      <c r="Q30" s="17">
+      <c r="Q30" s="16">
         <f t="shared" si="7"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="R30" s="17"/>
-      <c r="S30" s="18">
+      <c r="R30" s="16"/>
+      <c r="S30" s="17">
         <f>46.3+33.9*LOG(2000)+10*LOG($D$30/2000)-13.82*LOG(MAX(30,$I$30))+(44.9-6.55*LOG(MAX(30,$I$30)))*POWER((LOG($E$30)),$L$30)-$P$30-$Q$30</f>
         <v>116.85470194967921</v>
       </c>
-      <c r="T30" s="53"/>
+      <c r="T30" s="52"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
@@ -2062,11 +2235,11 @@
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J31" s="17">
+      <c r="J31" s="16">
         <f t="shared" si="4"/>
         <v>1.1278098829275329E-2</v>
       </c>
-      <c r="K31" s="17">
+      <c r="K31" s="16">
         <f t="shared" si="5"/>
         <v>-3.5218251811136252</v>
       </c>
@@ -2074,24 +2247,24 @@
         <v>1</v>
       </c>
       <c r="M31" s="6"/>
-      <c r="N31" s="64">
+      <c r="N31" s="63">
         <f>$S$25-2*POWER((LOG((MIN(MAX(150,$D$31),2000))/28)),2)-5.4</f>
         <v>94.49709568389251</v>
       </c>
-      <c r="P31" s="50">
+      <c r="P31" s="49">
         <f t="shared" si="6"/>
         <v>1.1278098829275329E-2</v>
       </c>
-      <c r="Q31" s="17">
+      <c r="Q31" s="16">
         <f t="shared" si="7"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="R31" s="17"/>
-      <c r="S31" s="18">
+      <c r="R31" s="16"/>
+      <c r="S31" s="17">
         <f>$S$25-2*POWER((LOG((MIN(MAX(150,$D$31),2000))/28)),2)-5.4</f>
         <v>94.49709568389251</v>
       </c>
-      <c r="T31" s="53"/>
+      <c r="T31" s="52"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
@@ -2123,11 +2296,11 @@
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J32" s="17">
+      <c r="J32" s="16">
         <f t="shared" si="4"/>
         <v>1.1278098829275329E-2</v>
       </c>
-      <c r="K32" s="17">
+      <c r="K32" s="16">
         <f t="shared" si="5"/>
         <v>-3.5218251811136252</v>
       </c>
@@ -2135,24 +2308,24 @@
         <v>1</v>
       </c>
       <c r="M32" s="6"/>
-      <c r="N32" s="64">
+      <c r="N32" s="63">
         <f>$S$26-2*POWER((LOG((MIN(MAX(150,$D$32),2000))/28)),2)-5.4</f>
         <v>94.49709568389251</v>
       </c>
-      <c r="P32" s="50">
+      <c r="P32" s="49">
         <f t="shared" si="6"/>
         <v>1.1278098829275329E-2</v>
       </c>
-      <c r="Q32" s="17">
+      <c r="Q32" s="16">
         <f t="shared" si="7"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="R32" s="17"/>
-      <c r="S32" s="18">
+      <c r="R32" s="16"/>
+      <c r="S32" s="17">
         <f>$S$26-2*POWER((LOG((MIN(MAX(150,$D$32),2000))/28)),2)-5.4</f>
         <v>94.49709568389251</v>
       </c>
-      <c r="T32" s="53"/>
+      <c r="T32" s="52"/>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
@@ -2184,11 +2357,11 @@
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J33" s="17">
+      <c r="J33" s="16">
         <f t="shared" si="4"/>
         <v>1.1278098829275329E-2</v>
       </c>
-      <c r="K33" s="17">
+      <c r="K33" s="16">
         <f t="shared" si="5"/>
         <v>-3.5218251811136252</v>
       </c>
@@ -2196,24 +2369,24 @@
         <v>1</v>
       </c>
       <c r="M33" s="6"/>
-      <c r="N33" s="64">
+      <c r="N33" s="63">
         <f>$S$36-2*POWER((LOG((MIN(MAX(150,$D$33),2000))/28)),2)-5.4</f>
         <v>108.5144750990882</v>
       </c>
-      <c r="P33" s="50">
+      <c r="P33" s="49">
         <f t="shared" si="6"/>
         <v>1.1278098829275329E-2</v>
       </c>
-      <c r="Q33" s="17">
+      <c r="Q33" s="16">
         <f t="shared" si="7"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="R33" s="17"/>
-      <c r="S33" s="18">
+      <c r="R33" s="16"/>
+      <c r="S33" s="17">
         <f>$S$36-2*POWER((LOG((MIN(MAX(150,$D$33),2000))/28)),2)-5.4</f>
         <v>108.5144750990882</v>
       </c>
-      <c r="T33" s="53"/>
+      <c r="T33" s="52"/>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
@@ -2245,11 +2418,11 @@
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J34" s="17">
+      <c r="J34" s="16">
         <f t="shared" si="4"/>
         <v>1.1278098829275329E-2</v>
       </c>
-      <c r="K34" s="17">
+      <c r="K34" s="16">
         <f t="shared" si="5"/>
         <v>-3.5218251811136252</v>
       </c>
@@ -2257,24 +2430,24 @@
         <v>1</v>
       </c>
       <c r="M34" s="6"/>
-      <c r="N34" s="64">
+      <c r="N34" s="63">
         <f>$S$37-2*POWER((LOG((MIN(MAX(150,$D$34),2000))/28)),2)-5.4</f>
         <v>108.5144750990882</v>
       </c>
-      <c r="P34" s="50">
+      <c r="P34" s="49">
         <f t="shared" si="6"/>
         <v>1.1278098829275329E-2</v>
       </c>
-      <c r="Q34" s="17">
+      <c r="Q34" s="16">
         <f t="shared" si="7"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="R34" s="17"/>
-      <c r="S34" s="18">
+      <c r="R34" s="16"/>
+      <c r="S34" s="17">
         <f>$S$37-2*POWER((LOG((MIN(MAX(150,$D$34),2000))/28)),2)-5.4</f>
         <v>108.5144750990882</v>
       </c>
-      <c r="T34" s="53"/>
+      <c r="T34" s="52"/>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
@@ -2306,11 +2479,11 @@
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J35" s="17">
+      <c r="J35" s="16">
         <f t="shared" si="4"/>
         <v>4.2974525459298363E-2</v>
       </c>
-      <c r="K35" s="17">
+      <c r="K35" s="16">
         <f t="shared" si="5"/>
         <v>-3.5218251811136252</v>
       </c>
@@ -2318,148 +2491,148 @@
         <v>1</v>
       </c>
       <c r="M35" s="6"/>
-      <c r="N35" s="64">
+      <c r="N35" s="63">
         <f>$S$27-4.78*POWER(LOG(   MIN( MAX(150, $D$35),2000) ),2)+18.33*LOG(MIN(MAX(150,$D$35),2000))-40.94</f>
         <v>83.17410064432147</v>
       </c>
-      <c r="P35" s="50">
+      <c r="P35" s="49">
         <f t="shared" si="6"/>
         <v>4.2974525459298363E-2</v>
       </c>
-      <c r="Q35" s="17">
+      <c r="Q35" s="16">
         <f t="shared" si="7"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="R35" s="17"/>
-      <c r="S35" s="18">
+      <c r="R35" s="16"/>
+      <c r="S35" s="17">
         <f>$S$27-4.78*POWER(LOG(   MIN( MAX(150, $D$35),2000) ),2)+18.33*LOG(MIN(MAX(150,$D$35),2000))-40.94</f>
         <v>83.17410064432147</v>
       </c>
-      <c r="T35" s="53"/>
+      <c r="T35" s="52"/>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A36" s="57" t="s">
+      <c r="A36" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="B36" s="58" t="s">
+      <c r="B36" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="58">
-        <v>1</v>
-      </c>
-      <c r="D36" s="58">
+      <c r="C36" s="57">
+        <v>1</v>
+      </c>
+      <c r="D36" s="57">
         <v>800</v>
       </c>
-      <c r="E36" s="58">
+      <c r="E36" s="57">
         <v>0.5</v>
       </c>
-      <c r="F36" s="58">
-        <v>20</v>
-      </c>
-      <c r="G36" s="58">
-        <v>1.5</v>
-      </c>
-      <c r="H36" s="58">
+      <c r="F36" s="57">
+        <v>20</v>
+      </c>
+      <c r="G36" s="57">
+        <v>1.5</v>
+      </c>
+      <c r="H36" s="57">
         <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
-      <c r="I36" s="58">
+      <c r="I36" s="57">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J36" s="59">
+      <c r="J36" s="58">
         <f t="shared" si="4"/>
         <v>1.1278098829275329E-2</v>
       </c>
-      <c r="K36" s="59">
+      <c r="K36" s="58">
         <f t="shared" si="5"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="L36" s="58">
-        <v>1</v>
-      </c>
-      <c r="M36" s="58"/>
-      <c r="N36" s="65">
+      <c r="L36" s="57">
+        <v>1</v>
+      </c>
+      <c r="M36" s="57"/>
+      <c r="N36" s="64">
         <f>69.6+26.2*LOG($D$36)-13.82*LOG(MAX(30,$I$36))+(44.9-6.55*LOG(MAX(30,$I$36)))*POWER((LOG($E$36)),$L$36)-$P$36-$Q$36</f>
         <v>118.15395081805227</v>
       </c>
-      <c r="O36" s="61"/>
-      <c r="P36" s="62">
+      <c r="O36" s="60"/>
+      <c r="P36" s="61">
         <f t="shared" si="6"/>
         <v>1.1278098829275329E-2</v>
       </c>
-      <c r="Q36" s="59">
+      <c r="Q36" s="58">
         <f t="shared" si="7"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="R36" s="59"/>
-      <c r="S36" s="60">
+      <c r="R36" s="58"/>
+      <c r="S36" s="59">
         <f>69.6+26.2*LOG($D$36)-13.82*LOG(MAX(30,$I$36))+(44.9-6.55*LOG(MAX(30,$I$36)))*POWER((LOG($E$36)),$L$36)-$P$36-$Q$36</f>
         <v>118.15395081805227</v>
       </c>
-      <c r="T36" s="53"/>
+      <c r="T36" s="52"/>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A37" s="57" t="s">
+      <c r="A37" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="B37" s="58" t="s">
+      <c r="B37" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="C37" s="58">
+      <c r="C37" s="57">
         <v>0</v>
       </c>
-      <c r="D37" s="58">
+      <c r="D37" s="57">
         <v>800</v>
       </c>
-      <c r="E37" s="58">
+      <c r="E37" s="57">
         <v>0.5</v>
       </c>
-      <c r="F37" s="58">
-        <v>20</v>
-      </c>
-      <c r="G37" s="58">
-        <v>1.5</v>
-      </c>
-      <c r="H37" s="58">
+      <c r="F37" s="57">
+        <v>20</v>
+      </c>
+      <c r="G37" s="57">
+        <v>1.5</v>
+      </c>
+      <c r="H37" s="57">
         <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
-      <c r="I37" s="58">
+      <c r="I37" s="57">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J37" s="59">
+      <c r="J37" s="58">
         <f t="shared" si="4"/>
         <v>1.1278098829275329E-2</v>
       </c>
-      <c r="K37" s="59">
+      <c r="K37" s="58">
         <f t="shared" si="5"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="L37" s="58">
-        <v>1</v>
-      </c>
-      <c r="M37" s="58"/>
-      <c r="N37" s="65">
+      <c r="L37" s="57">
+        <v>1</v>
+      </c>
+      <c r="M37" s="57"/>
+      <c r="N37" s="64">
         <f>69.6+26.2*LOG($D$37)-13.82*LOG(MAX(30,$I$37))+(44.9-6.55*LOG(MAX(30,$I$37)))*POWER((LOG($E$37)),$L$37)-$P$37-$Q$37</f>
         <v>118.15395081805227</v>
       </c>
-      <c r="O37" s="61"/>
-      <c r="P37" s="62">
+      <c r="O37" s="60"/>
+      <c r="P37" s="61">
         <f t="shared" si="6"/>
         <v>1.1278098829275329E-2</v>
       </c>
-      <c r="Q37" s="59">
+      <c r="Q37" s="58">
         <f t="shared" si="7"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="R37" s="59"/>
-      <c r="S37" s="60">
+      <c r="R37" s="58"/>
+      <c r="S37" s="59">
         <f>69.6+26.2*LOG($D$37)-13.82*LOG(MAX(30,$I$37))+(44.9-6.55*LOG(MAX(30,$I$37)))*POWER((LOG($E$37)),$L$37)-$P$37-$Q$37</f>
         <v>118.15395081805227</v>
       </c>
-      <c r="T37" s="53"/>
+      <c r="T37" s="52"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
@@ -2491,11 +2664,11 @@
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J38" s="17">
+      <c r="J38" s="16">
         <f t="shared" si="4"/>
         <v>4.2974525459298363E-2</v>
       </c>
-      <c r="K38" s="17">
+      <c r="K38" s="16">
         <f t="shared" si="5"/>
         <v>-3.5218251811136252</v>
       </c>
@@ -2503,24 +2676,24 @@
         <v>1</v>
       </c>
       <c r="M38" s="6"/>
-      <c r="N38" s="64">
+      <c r="N38" s="63">
         <f>46.3+33.9*LOG($D$38)-13.82*LOG(MAX(30,$I$38))+(44.9-6.55*LOG(MAX(30,$I$38)))*POWER((LOG($E$38)),$L$38)-$P$38-$Q$38</f>
         <v>129.11503465523538</v>
       </c>
-      <c r="P38" s="50">
+      <c r="P38" s="49">
         <f t="shared" si="6"/>
         <v>4.2974525459298363E-2</v>
       </c>
-      <c r="Q38" s="17">
+      <c r="Q38" s="16">
         <f t="shared" si="7"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="R38" s="17"/>
-      <c r="S38" s="18">
+      <c r="R38" s="16"/>
+      <c r="S38" s="17">
         <f>46.3+33.9*LOG($D$38)-13.82*LOG(MAX(30,$I$38))+(44.9-6.55*LOG(MAX(30,$I$38)))*POWER((LOG($E$38)),$L$38)-$P$38-$Q$38</f>
         <v>129.11503465523538</v>
       </c>
-      <c r="T38" s="53"/>
+      <c r="T38" s="52"/>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
@@ -2552,11 +2725,11 @@
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J39" s="17">
+      <c r="J39" s="16">
         <f t="shared" si="4"/>
         <v>4.2974525459298363E-2</v>
       </c>
-      <c r="K39" s="17">
+      <c r="K39" s="16">
         <f t="shared" si="5"/>
         <v>-3.5218251811136252</v>
       </c>
@@ -2564,27 +2737,27 @@
         <v>1</v>
       </c>
       <c r="M39" s="6"/>
-      <c r="N39" s="64">
+      <c r="N39" s="63">
         <f>46.3+33.9*LOG($D$39)-13.82*LOG(MAX(30,$I$39))+(44.9-6.55*LOG(MAX(30,$I$39)))*POWER((LOG($E$39)),$L$39)-$P$39-$Q$39</f>
         <v>129.11503465523538</v>
       </c>
-      <c r="P39" s="50">
+      <c r="P39" s="49">
         <f t="shared" si="6"/>
         <v>4.2974525459298363E-2</v>
       </c>
-      <c r="Q39" s="17">
+      <c r="Q39" s="16">
         <f t="shared" si="7"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="R39" s="17"/>
-      <c r="S39" s="18">
+      <c r="R39" s="16"/>
+      <c r="S39" s="17">
         <f>46.3+33.9*LOG($D$39)-13.82*LOG(MAX(30,$I$39))+(44.9-6.55*LOG(MAX(30,$I$39)))*POWER((LOG($E$39)),$L$39)-$P$39-$Q$39</f>
         <v>129.11503465523538</v>
       </c>
-      <c r="T39" s="53"/>
+      <c r="T39" s="52"/>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A40" s="20" t="s">
+      <c r="A40" s="19" t="s">
         <v>20</v>
       </c>
       <c r="B40" s="6" t="s">
@@ -2613,11 +2786,11 @@
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J40" s="17">
+      <c r="J40" s="16">
         <f t="shared" si="4"/>
         <v>4.2974525459298363E-2</v>
       </c>
-      <c r="K40" s="17">
+      <c r="K40" s="16">
         <f t="shared" si="5"/>
         <v>-3.5218251811136252</v>
       </c>
@@ -2625,27 +2798,27 @@
         <v>1</v>
       </c>
       <c r="M40" s="6"/>
-      <c r="N40" s="64">
+      <c r="N40" s="63">
         <f>32.4+(20*LOG($D$40))+(10*LOG(POWER($E$40,2)+POWER(($I$40-$H$40),2)/(POWER(10,6))))</f>
         <v>77.651600418352942</v>
       </c>
-      <c r="P40" s="50">
+      <c r="P40" s="49">
         <f t="shared" si="6"/>
         <v>4.2974525459298363E-2</v>
       </c>
-      <c r="Q40" s="17">
+      <c r="Q40" s="16">
         <f t="shared" si="7"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="R40" s="17"/>
-      <c r="S40" s="18">
+      <c r="R40" s="16"/>
+      <c r="S40" s="17">
         <f>32.4+(20*LOG($D$40))+(10*LOG(POWER($E$40,2)+POWER(($I$40-$H$40),2)/(POWER(10,6))))</f>
         <v>77.651600418352942</v>
       </c>
-      <c r="T40" s="53"/>
+      <c r="T40" s="52"/>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A41" s="20" t="s">
+      <c r="A41" s="19" t="s">
         <v>20</v>
       </c>
       <c r="B41" s="6" t="s">
@@ -2674,11 +2847,11 @@
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J41" s="17">
+      <c r="J41" s="16">
         <f t="shared" si="4"/>
         <v>4.2974525459298363E-2</v>
       </c>
-      <c r="K41" s="17">
+      <c r="K41" s="16">
         <f t="shared" si="5"/>
         <v>-3.5218251811136252</v>
       </c>
@@ -2686,27 +2859,27 @@
         <v>1</v>
       </c>
       <c r="M41" s="6"/>
-      <c r="N41" s="64">
+      <c r="N41" s="63">
         <f>32.4+(20*LOG($D$41))+(10*LOG(POWER($E$41,2)+POWER(($I$41-$H$41),2)/(POWER(10,6))))</f>
         <v>70.388501403267725</v>
       </c>
-      <c r="P41" s="50">
+      <c r="P41" s="49">
         <f t="shared" si="6"/>
         <v>4.2974525459298363E-2</v>
       </c>
-      <c r="Q41" s="17">
+      <c r="Q41" s="16">
         <f t="shared" si="7"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="R41" s="17"/>
-      <c r="S41" s="18">
+      <c r="R41" s="16"/>
+      <c r="S41" s="17">
         <f>32.4+(20*LOG($D$41))+(10*LOG(POWER($E$41,2)+POWER(($I$41-$H$41),2)/(POWER(10,6))))</f>
         <v>70.388501403267725</v>
       </c>
-      <c r="T41" s="53"/>
+      <c r="T41" s="52"/>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A42" s="20" t="s">
+      <c r="A42" s="19" t="s">
         <v>20</v>
       </c>
       <c r="B42" s="6" t="s">
@@ -2735,11 +2908,11 @@
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J42" s="17">
+      <c r="J42" s="16">
         <f t="shared" si="4"/>
         <v>4.2974525459298363E-2</v>
       </c>
-      <c r="K42" s="17">
+      <c r="K42" s="16">
         <f t="shared" si="5"/>
         <v>-3.5218251811136252</v>
       </c>
@@ -2747,27 +2920,27 @@
         <v>1</v>
       </c>
       <c r="M42" s="6"/>
-      <c r="N42" s="64">
+      <c r="N42" s="63">
         <f>N41+(LOG($E$42)-LOG(0.04))/(LOG(0.1)-LOG(0.04))*($S$40-$S$41)</f>
         <v>76.816446431868741</v>
       </c>
-      <c r="P42" s="50">
+      <c r="P42" s="49">
         <f t="shared" si="6"/>
         <v>4.2974525459298363E-2</v>
       </c>
-      <c r="Q42" s="17">
+      <c r="Q42" s="16">
         <f t="shared" si="7"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="R42" s="17"/>
-      <c r="S42" s="18">
+      <c r="R42" s="16"/>
+      <c r="S42" s="17">
         <f>S41+(LOG($E$42)-LOG(0.04))/(LOG(0.1)-LOG(0.04))*($S$40-$S$41)</f>
         <v>76.816446431868741</v>
       </c>
-      <c r="T42" s="53"/>
+      <c r="T42" s="52"/>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A43" s="20" t="s">
+      <c r="A43" s="19" t="s">
         <v>20</v>
       </c>
       <c r="B43" s="6" t="s">
@@ -2796,11 +2969,11 @@
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J43" s="17">
+      <c r="J43" s="16">
         <f t="shared" si="4"/>
         <v>4.2974525459298363E-2</v>
       </c>
-      <c r="K43" s="17">
+      <c r="K43" s="16">
         <f t="shared" si="5"/>
         <v>-3.5218251811136252</v>
       </c>
@@ -2808,87 +2981,87 @@
         <v>1</v>
       </c>
       <c r="M43" s="6"/>
-      <c r="N43" s="64">
+      <c r="N43" s="63">
         <f>$S$41+(LOG($E$43)-LOG(0.04))/(LOG(0.1)-LOG(0.04))*($S$40-$S$41)</f>
         <v>76.816446431868741</v>
       </c>
-      <c r="P43" s="50">
+      <c r="P43" s="49">
         <f t="shared" si="6"/>
         <v>4.2974525459298363E-2</v>
       </c>
-      <c r="Q43" s="17">
+      <c r="Q43" s="16">
         <f t="shared" si="7"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="R43" s="17"/>
-      <c r="S43" s="18">
+      <c r="R43" s="16"/>
+      <c r="S43" s="17">
         <f>$S$41+(LOG($E$43)-LOG(0.04))/(LOG(0.1)-LOG(0.04))*($S$40-$S$41)</f>
         <v>76.816446431868741</v>
       </c>
-      <c r="T43" s="53"/>
-    </row>
-    <row r="44" spans="1:20" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="21" t="s">
+      <c r="T43" s="52"/>
+    </row>
+    <row r="44" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B44" s="22" t="s">
+      <c r="B44" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C44" s="22">
-        <v>1</v>
-      </c>
-      <c r="D44" s="22">
+      <c r="C44" s="21">
+        <v>1</v>
+      </c>
+      <c r="D44" s="21">
         <v>1800</v>
       </c>
-      <c r="E44" s="22">
+      <c r="E44" s="21">
         <v>5</v>
       </c>
-      <c r="F44" s="22">
-        <v>20</v>
-      </c>
-      <c r="G44" s="22">
-        <v>1.5</v>
-      </c>
-      <c r="H44" s="22">
+      <c r="F44" s="21">
+        <v>20</v>
+      </c>
+      <c r="G44" s="21">
+        <v>1.5</v>
+      </c>
+      <c r="H44" s="21">
         <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
-      <c r="I44" s="22">
+      <c r="I44" s="21">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J44" s="17">
+      <c r="J44" s="16">
         <f t="shared" si="4"/>
         <v>4.2974525459298363E-2</v>
       </c>
-      <c r="K44" s="17">
+      <c r="K44" s="16">
         <f t="shared" si="5"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="L44" s="22">
-        <v>1</v>
-      </c>
-      <c r="M44" s="22"/>
-      <c r="N44" s="66">
+      <c r="L44" s="21">
+        <v>1</v>
+      </c>
+      <c r="M44" s="21"/>
+      <c r="N44" s="65">
         <f>46.3+33.9*LOG($D$44)-13.82*LOG(MAX(30,$I$44))+(44.9-6.55*LOG(MAX(30,$I$44)))*POWER((LOG($E$44)),$L$44)-$P$44-$Q$44</f>
         <v>164.33989043682161</v>
       </c>
-      <c r="P44" s="50">
+      <c r="P44" s="49">
         <f t="shared" si="6"/>
         <v>4.2974525459298363E-2</v>
       </c>
-      <c r="Q44" s="17">
+      <c r="Q44" s="16">
         <f t="shared" si="7"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="R44" s="17"/>
-      <c r="S44" s="23">
+      <c r="R44" s="16"/>
+      <c r="S44" s="22">
         <f>46.3+33.9*LOG($D$44)-13.82*LOG(MAX(30,$I$44))+(44.9-6.55*LOG(MAX(30,$I$44)))*POWER((LOG($E$44)),$L$44)-$P$44-$Q$44</f>
         <v>164.33989043682161</v>
       </c>
-      <c r="T44" s="53"/>
-    </row>
-    <row r="45" spans="1:20" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="T44" s="52"/>
+    </row>
+    <row r="45" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>17</v>
       </c>
@@ -2918,11 +3091,11 @@
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J45" s="17">
+      <c r="J45" s="16">
         <f t="shared" si="4"/>
         <v>4.2974525459298363E-2</v>
       </c>
-      <c r="K45" s="17">
+      <c r="K45" s="16">
         <f t="shared" si="5"/>
         <v>-3.5218251811136252</v>
       </c>
@@ -2930,1113 +3103,1113 @@
         <v>1</v>
       </c>
       <c r="M45" s="6"/>
-      <c r="N45" s="64">
+      <c r="N45" s="63">
         <f>$S$44-4.78*POWER(LOG(   MIN( MAX(150, $D$45),2000)),2)+18.33*LOG(MIN(MAX(150,$D$45),2000))-40.94</f>
         <v>132.41633584110338</v>
       </c>
-      <c r="P45" s="50">
+      <c r="P45" s="49">
         <f t="shared" si="6"/>
         <v>4.2974525459298363E-2</v>
       </c>
-      <c r="Q45" s="17">
+      <c r="Q45" s="16">
         <f t="shared" si="7"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="R45" s="17"/>
-      <c r="S45" s="18">
+      <c r="R45" s="16"/>
+      <c r="S45" s="17">
         <f>$S$44-4.78*POWER(LOG(   MIN( MAX(150, $D$45),2000)),2)+18.33*LOG(MIN(MAX(150,$D$45),2000))-40.94</f>
         <v>132.41633584110338</v>
       </c>
-      <c r="T45" s="53"/>
-    </row>
-    <row r="46" spans="1:20" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="25" t="s">
+      <c r="T45" s="52"/>
+    </row>
+    <row r="46" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B46" s="26" t="s">
+      <c r="B46" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C46" s="26">
-        <v>1</v>
-      </c>
-      <c r="D46" s="26">
+      <c r="C46" s="25">
+        <v>1</v>
+      </c>
+      <c r="D46" s="25">
         <v>700</v>
       </c>
-      <c r="E46" s="26">
-        <v>20</v>
-      </c>
-      <c r="F46" s="26">
-        <v>20</v>
-      </c>
-      <c r="G46" s="26">
-        <v>1.5</v>
-      </c>
-      <c r="H46" s="26">
+      <c r="E46" s="25">
+        <v>20</v>
+      </c>
+      <c r="F46" s="25">
+        <v>20</v>
+      </c>
+      <c r="G46" s="25">
+        <v>1.5</v>
+      </c>
+      <c r="H46" s="25">
         <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
-      <c r="I46" s="26">
+      <c r="I46" s="25">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J46" s="17">
+      <c r="J46" s="16">
         <f t="shared" si="4"/>
         <v>6.0588236012835139E-3</v>
       </c>
-      <c r="K46" s="17">
+      <c r="K46" s="16">
         <f t="shared" si="5"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="L46" s="26">
-        <v>1</v>
-      </c>
-      <c r="M46" s="27"/>
-      <c r="N46" s="64">
+      <c r="L46" s="25">
+        <v>1</v>
+      </c>
+      <c r="M46" s="26"/>
+      <c r="N46" s="63">
         <f>69.6+26.2*LOG($D$46)-13.82*LOG(MAX(30,$I$46))+(44.9-6.55*LOG(MAX(30,$I$46)))*POWER(LOG($E$46),$L$46)-$P$46-$Q$46</f>
         <v>173.07211323044163</v>
       </c>
-      <c r="P46" s="50">
+      <c r="P46" s="49">
         <f t="shared" si="6"/>
         <v>6.0588236012835139E-3</v>
       </c>
-      <c r="Q46" s="17">
+      <c r="Q46" s="16">
         <f t="shared" si="7"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="R46" s="17"/>
-      <c r="S46" s="28">
+      <c r="R46" s="16"/>
+      <c r="S46" s="27">
         <f>69.6+26.2*LOG($D$46)-13.82*LOG(MAX(30,$I$46))+(44.9-6.55*LOG(MAX(30,$I$46)))*POWER(LOG($E$46),$L$46)-$P$46-$Q$46</f>
         <v>173.07211323044163</v>
       </c>
-      <c r="T46" s="53"/>
-    </row>
-    <row r="47" spans="1:20" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="25" t="s">
+      <c r="T46" s="52"/>
+    </row>
+    <row r="47" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B47" s="26" t="s">
+      <c r="B47" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C47" s="26">
-        <v>1</v>
-      </c>
-      <c r="D47" s="26">
+      <c r="C47" s="25">
+        <v>1</v>
+      </c>
+      <c r="D47" s="25">
         <v>700</v>
       </c>
-      <c r="E47" s="26">
-        <v>20</v>
-      </c>
-      <c r="F47" s="26">
-        <v>20</v>
-      </c>
-      <c r="G47" s="26">
-        <v>1.5</v>
-      </c>
-      <c r="H47" s="26">
+      <c r="E47" s="25">
+        <v>20</v>
+      </c>
+      <c r="F47" s="25">
+        <v>20</v>
+      </c>
+      <c r="G47" s="25">
+        <v>1.5</v>
+      </c>
+      <c r="H47" s="25">
         <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
-      <c r="I47" s="26">
+      <c r="I47" s="25">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J47" s="17">
+      <c r="J47" s="16">
         <f t="shared" si="4"/>
         <v>6.0588236012835139E-3</v>
       </c>
-      <c r="K47" s="17">
+      <c r="K47" s="16">
         <f t="shared" si="5"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="L47" s="26">
-        <v>1</v>
-      </c>
-      <c r="M47" s="27"/>
-      <c r="N47" s="64">
+      <c r="L47" s="25">
+        <v>1</v>
+      </c>
+      <c r="M47" s="26"/>
+      <c r="N47" s="63">
         <f>$S$46-4.78*POWER(LOG(   MIN( MAX(150, $D$47),2000) ),2)+18.33*LOG(MIN(MAX(150,$D$47),2000))-40.94</f>
         <v>145.59065424604259</v>
       </c>
-      <c r="P47" s="50">
+      <c r="P47" s="49">
         <f t="shared" si="6"/>
         <v>6.0588236012835139E-3</v>
       </c>
-      <c r="Q47" s="17">
+      <c r="Q47" s="16">
         <f t="shared" si="7"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="R47" s="17"/>
-      <c r="S47" s="28">
+      <c r="R47" s="16"/>
+      <c r="S47" s="27">
         <f>$S$46-4.78*POWER(LOG(   MIN( MAX(150, $D$47),2000) ),2)+18.33*LOG(MIN(MAX(150,$D$47),2000))-40.94</f>
         <v>145.59065424604259</v>
       </c>
-      <c r="T47" s="53"/>
-    </row>
-    <row r="48" spans="1:20" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="25" t="s">
+      <c r="T47" s="52"/>
+    </row>
+    <row r="48" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B48" s="26" t="s">
+      <c r="B48" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C48" s="26">
-        <v>1</v>
-      </c>
-      <c r="D48" s="26">
+      <c r="C48" s="25">
+        <v>1</v>
+      </c>
+      <c r="D48" s="25">
         <v>700</v>
       </c>
-      <c r="E48" s="26">
+      <c r="E48" s="25">
         <v>21</v>
       </c>
-      <c r="F48" s="26">
-        <v>20</v>
-      </c>
-      <c r="G48" s="26">
-        <v>1.5</v>
-      </c>
-      <c r="H48" s="26">
+      <c r="F48" s="25">
+        <v>20</v>
+      </c>
+      <c r="G48" s="25">
+        <v>1.5</v>
+      </c>
+      <c r="H48" s="25">
         <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
-      <c r="I48" s="26">
+      <c r="I48" s="25">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J48" s="17">
+      <c r="J48" s="16">
         <f t="shared" si="4"/>
         <v>6.0588236012835139E-3</v>
       </c>
-      <c r="K48" s="17">
+      <c r="K48" s="16">
         <f t="shared" si="5"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="L48" s="26"/>
-      <c r="M48" s="27">
+      <c r="L48" s="25"/>
+      <c r="M48" s="26">
         <f>1+(0.14+0.000187*$D48+0.00107*$I48)*POWER(LOG($E48/20),0.8)</f>
         <v>1.0133881968090026</v>
       </c>
-      <c r="N48" s="64">
+      <c r="N48" s="63">
         <f>69.6+26.2*LOG($D$48)-13.82*LOG(MAX(30,$I$48))+(44.9-6.55*LOG(MAX(30,$I$48)))*POWER(LOG($E$48),$R$48)-$P$48-$Q$48</f>
         <v>173.99299545055089</v>
       </c>
-      <c r="P48" s="50">
+      <c r="P48" s="49">
         <f t="shared" si="6"/>
         <v>6.0588236012835139E-3</v>
       </c>
-      <c r="Q48" s="17">
+      <c r="Q48" s="16">
         <f t="shared" si="7"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="R48" s="27">
+      <c r="R48" s="26">
         <f>1+(0.14+0.000187*$D48+0.00107*$I48)*POWER(LOG($E48/20),0.8)</f>
         <v>1.0133881968090026</v>
       </c>
-      <c r="S48" s="28">
+      <c r="S48" s="27">
         <f>69.6+26.2*LOG($D$48)-13.82*LOG(MAX(30,$I$48))+(44.9-6.55*LOG(MAX(30,$I$48)))*POWER(LOG($E$48),$R$48)-$P$48-$Q$48</f>
         <v>173.99299545055089</v>
       </c>
-      <c r="T48" s="53"/>
-    </row>
-    <row r="49" spans="1:20" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="25" t="s">
+      <c r="T48" s="52"/>
+    </row>
+    <row r="49" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B49" s="26" t="s">
+      <c r="B49" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C49" s="26">
-        <v>1</v>
-      </c>
-      <c r="D49" s="26">
+      <c r="C49" s="25">
+        <v>1</v>
+      </c>
+      <c r="D49" s="25">
         <v>700</v>
       </c>
-      <c r="E49" s="26">
+      <c r="E49" s="25">
         <v>21</v>
       </c>
-      <c r="F49" s="26">
-        <v>20</v>
-      </c>
-      <c r="G49" s="26">
-        <v>1.5</v>
-      </c>
-      <c r="H49" s="26">
+      <c r="F49" s="25">
+        <v>20</v>
+      </c>
+      <c r="G49" s="25">
+        <v>1.5</v>
+      </c>
+      <c r="H49" s="25">
         <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
-      <c r="I49" s="26">
+      <c r="I49" s="25">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J49" s="17">
+      <c r="J49" s="16">
         <f t="shared" si="4"/>
         <v>6.0588236012835139E-3</v>
       </c>
-      <c r="K49" s="17">
+      <c r="K49" s="16">
         <f t="shared" si="5"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="L49" s="26"/>
-      <c r="M49" s="27">
+      <c r="L49" s="25"/>
+      <c r="M49" s="26">
         <f t="shared" ref="M49:M53" si="8">1+(0.14+0.000187*$D49+0.00107*$I49)*POWER(LOG($E49/20),0.8)</f>
         <v>1.0133881968090026</v>
       </c>
-      <c r="N49" s="64">
+      <c r="N49" s="63">
         <f>$S$48-4.78*POWER(LOG(   MIN( MAX(150, $D$49),2000) ),2)+18.33*LOG(MIN(MAX(150,$D$49),2000))-40.94</f>
         <v>146.51153646615185</v>
       </c>
-      <c r="P49" s="50">
+      <c r="P49" s="49">
         <f t="shared" si="6"/>
         <v>6.0588236012835139E-3</v>
       </c>
-      <c r="Q49" s="17">
+      <c r="Q49" s="16">
         <f t="shared" si="7"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="R49" s="27">
+      <c r="R49" s="26">
         <f t="shared" ref="R49:R53" si="9">1+(0.14+0.000187*$D49+0.00107*$I49)*POWER(LOG($E49/20),0.8)</f>
         <v>1.0133881968090026</v>
       </c>
-      <c r="S49" s="28">
+      <c r="S49" s="27">
         <f>$S$48-4.78*POWER(LOG(   MIN( MAX(150, $D$49),2000) ),2)+18.33*LOG(MIN(MAX(150,$D$49),2000))-40.94</f>
         <v>146.51153646615185</v>
       </c>
-      <c r="T49" s="53"/>
-    </row>
-    <row r="50" spans="1:20" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="25" t="s">
+      <c r="T49" s="52"/>
+    </row>
+    <row r="50" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B50" s="26" t="s">
+      <c r="B50" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C50" s="26">
-        <v>1</v>
-      </c>
-      <c r="D50" s="26">
+      <c r="C50" s="25">
+        <v>1</v>
+      </c>
+      <c r="D50" s="25">
         <v>700</v>
       </c>
-      <c r="E50" s="26">
+      <c r="E50" s="25">
         <v>25</v>
       </c>
-      <c r="F50" s="26">
-        <v>20</v>
-      </c>
-      <c r="G50" s="26">
-        <v>1.5</v>
-      </c>
-      <c r="H50" s="26">
+      <c r="F50" s="25">
+        <v>20</v>
+      </c>
+      <c r="G50" s="25">
+        <v>1.5</v>
+      </c>
+      <c r="H50" s="25">
         <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
-      <c r="I50" s="26">
+      <c r="I50" s="25">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J50" s="17">
+      <c r="J50" s="16">
         <f t="shared" si="4"/>
         <v>6.0588236012835139E-3</v>
       </c>
-      <c r="K50" s="17">
+      <c r="K50" s="16">
         <f t="shared" si="5"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="L50" s="26"/>
-      <c r="M50" s="27">
+      <c r="L50" s="25"/>
+      <c r="M50" s="26">
         <f t="shared" si="8"/>
         <v>1.0451776604355734</v>
       </c>
-      <c r="N50" s="64">
+      <c r="N50" s="63">
         <f>69.6+26.2*LOG($D$50)-13.82*LOG(MAX(30,$I$50))+(44.9-6.55*LOG(MAX(30,$I$50)))*POWER(LOG($E$50),$R$50)-$P$50-$Q$50</f>
         <v>177.23667937644004</v>
       </c>
-      <c r="P50" s="50">
+      <c r="P50" s="49">
         <f t="shared" si="6"/>
         <v>6.0588236012835139E-3</v>
       </c>
-      <c r="Q50" s="17">
+      <c r="Q50" s="16">
         <f t="shared" si="7"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="R50" s="27">
+      <c r="R50" s="26">
         <f t="shared" si="9"/>
         <v>1.0451776604355734</v>
       </c>
-      <c r="S50" s="28">
+      <c r="S50" s="27">
         <f>69.6+26.2*LOG($D$50)-13.82*LOG(MAX(30,$I$50))+(44.9-6.55*LOG(MAX(30,$I$50)))*POWER(LOG($E$50),$R$50)-$P$50-$Q$50</f>
         <v>177.23667937644004</v>
       </c>
-      <c r="T50" s="53"/>
-    </row>
-    <row r="51" spans="1:20" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="25" t="s">
+      <c r="T50" s="52"/>
+    </row>
+    <row r="51" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B51" s="26" t="s">
+      <c r="B51" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C51" s="26">
-        <v>1</v>
-      </c>
-      <c r="D51" s="26">
+      <c r="C51" s="25">
+        <v>1</v>
+      </c>
+      <c r="D51" s="25">
         <v>700</v>
       </c>
-      <c r="E51" s="26">
+      <c r="E51" s="25">
         <v>25</v>
       </c>
-      <c r="F51" s="26">
-        <v>20</v>
-      </c>
-      <c r="G51" s="26">
-        <v>1.5</v>
-      </c>
-      <c r="H51" s="26">
+      <c r="F51" s="25">
+        <v>20</v>
+      </c>
+      <c r="G51" s="25">
+        <v>1.5</v>
+      </c>
+      <c r="H51" s="25">
         <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
-      <c r="I51" s="26">
+      <c r="I51" s="25">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J51" s="17">
+      <c r="J51" s="16">
         <f t="shared" si="4"/>
         <v>6.0588236012835139E-3</v>
       </c>
-      <c r="K51" s="17">
+      <c r="K51" s="16">
         <f t="shared" si="5"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="L51" s="26"/>
-      <c r="M51" s="27">
+      <c r="L51" s="25"/>
+      <c r="M51" s="26">
         <f t="shared" si="8"/>
         <v>1.0451776604355734</v>
       </c>
-      <c r="N51" s="64">
+      <c r="N51" s="63">
         <f>$S$50-4.78*POWER(LOG(   MIN( MAX(150, $D$51),2000) ),2)+18.33*LOG(MIN(MAX(150,$D$51),2000))-40.94</f>
         <v>149.755220392041</v>
       </c>
-      <c r="P51" s="50">
+      <c r="P51" s="49">
         <f t="shared" si="6"/>
         <v>6.0588236012835139E-3</v>
       </c>
-      <c r="Q51" s="17">
+      <c r="Q51" s="16">
         <f t="shared" si="7"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="R51" s="27">
+      <c r="R51" s="26">
         <f t="shared" si="9"/>
         <v>1.0451776604355734</v>
       </c>
-      <c r="S51" s="28">
+      <c r="S51" s="27">
         <f>$S$50-4.78*POWER(LOG(   MIN( MAX(150, $D$51),2000) ),2)+18.33*LOG(MIN(MAX(150,$D$51),2000))-40.94</f>
         <v>149.755220392041</v>
       </c>
-      <c r="T51" s="53"/>
-    </row>
-    <row r="52" spans="1:20" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="25" t="s">
+      <c r="T51" s="52"/>
+    </row>
+    <row r="52" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B52" s="26" t="s">
+      <c r="B52" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C52" s="26">
-        <v>1</v>
-      </c>
-      <c r="D52" s="26">
+      <c r="C52" s="25">
+        <v>1</v>
+      </c>
+      <c r="D52" s="25">
         <v>700</v>
       </c>
-      <c r="E52" s="26">
+      <c r="E52" s="25">
         <v>50</v>
       </c>
-      <c r="F52" s="26">
-        <v>20</v>
-      </c>
-      <c r="G52" s="26">
-        <v>1.5</v>
-      </c>
-      <c r="H52" s="26">
+      <c r="F52" s="25">
+        <v>20</v>
+      </c>
+      <c r="G52" s="25">
+        <v>1.5</v>
+      </c>
+      <c r="H52" s="25">
         <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
-      <c r="I52" s="26">
+      <c r="I52" s="25">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J52" s="17">
+      <c r="J52" s="16">
         <f t="shared" si="4"/>
         <v>6.0588236012835139E-3</v>
       </c>
-      <c r="K52" s="17">
+      <c r="K52" s="16">
         <f t="shared" si="5"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="L52" s="26"/>
-      <c r="M52" s="27">
+      <c r="L52" s="25"/>
+      <c r="M52" s="26">
         <f t="shared" si="8"/>
         <v>1.1398565785362531</v>
       </c>
-      <c r="N52" s="64">
+      <c r="N52" s="63">
         <f>69.6+26.2*LOG($D$52)-13.82*LOG(MAX(30,$I$52))+(44.9-6.55*LOG(MAX(30,$I$52)))*POWER(LOG($E$52),$R$52)-$P$52-$Q$52</f>
         <v>191.69426118849938</v>
       </c>
-      <c r="P52" s="50">
+      <c r="P52" s="49">
         <f t="shared" si="6"/>
         <v>6.0588236012835139E-3</v>
       </c>
-      <c r="Q52" s="17">
+      <c r="Q52" s="16">
         <f t="shared" si="7"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="R52" s="27">
+      <c r="R52" s="26">
         <f t="shared" si="9"/>
         <v>1.1398565785362531</v>
       </c>
-      <c r="S52" s="28">
+      <c r="S52" s="27">
         <f>69.6+26.2*LOG($D$52)-13.82*LOG(MAX(30,$I$52))+(44.9-6.55*LOG(MAX(30,$I$52)))*POWER(LOG($E$52),$R$52)-$P$52-$Q$52</f>
         <v>191.69426118849938</v>
       </c>
-      <c r="T52" s="53"/>
-    </row>
-    <row r="53" spans="1:20" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="29" t="s">
+      <c r="T52" s="52"/>
+    </row>
+    <row r="53" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B53" s="30" t="s">
+      <c r="B53" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C53" s="30">
-        <v>1</v>
-      </c>
-      <c r="D53" s="30">
+      <c r="C53" s="29">
+        <v>1</v>
+      </c>
+      <c r="D53" s="29">
         <v>700</v>
       </c>
-      <c r="E53" s="30">
+      <c r="E53" s="29">
         <v>50</v>
       </c>
-      <c r="F53" s="30">
-        <v>20</v>
-      </c>
-      <c r="G53" s="30">
-        <v>1.5</v>
-      </c>
-      <c r="H53" s="30">
+      <c r="F53" s="29">
+        <v>20</v>
+      </c>
+      <c r="G53" s="29">
+        <v>1.5</v>
+      </c>
+      <c r="H53" s="29">
         <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
-      <c r="I53" s="30">
+      <c r="I53" s="29">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J53" s="52">
+      <c r="J53" s="51">
         <f t="shared" si="4"/>
         <v>6.0588236012835139E-3</v>
       </c>
-      <c r="K53" s="52">
+      <c r="K53" s="51">
         <f t="shared" si="5"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="L53" s="30"/>
-      <c r="M53" s="31">
+      <c r="L53" s="29"/>
+      <c r="M53" s="30">
         <f t="shared" si="8"/>
         <v>1.1398565785362531</v>
       </c>
-      <c r="N53" s="67">
+      <c r="N53" s="66">
         <f>$S$52-4.78*POWER(LOG(   MIN( MAX(150, $D$53),2000) ),2)+18.33*LOG(MIN(MAX(150,$D$53),2000))-40.94</f>
         <v>164.21280220410034</v>
       </c>
-      <c r="P53" s="51">
+      <c r="P53" s="50">
         <f t="shared" si="6"/>
         <v>6.0588236012835139E-3</v>
       </c>
-      <c r="Q53" s="52">
+      <c r="Q53" s="51">
         <f t="shared" si="7"/>
         <v>-3.5218251811136252</v>
       </c>
-      <c r="R53" s="31">
+      <c r="R53" s="30">
         <f t="shared" si="9"/>
         <v>1.1398565785362531</v>
       </c>
-      <c r="S53" s="32">
+      <c r="S53" s="31">
         <f>$S$52-4.78*POWER(LOG(   MIN( MAX(150, $D$53),2000) ),2)+18.33*LOG(MIN(MAX(150,$D$53),2000))-40.94</f>
         <v>164.21280220410034</v>
       </c>
-      <c r="T53" s="53"/>
-    </row>
-    <row r="54" spans="1:20" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="26"/>
-      <c r="B54" s="26"/>
-      <c r="C54" s="26"/>
-      <c r="D54" s="26"/>
-      <c r="E54" s="26"/>
-      <c r="F54" s="26"/>
-      <c r="G54" s="26"/>
-      <c r="H54" s="26"/>
-      <c r="I54" s="26"/>
-      <c r="J54" s="17"/>
-      <c r="K54" s="17"/>
-      <c r="L54" s="26"/>
-      <c r="M54" s="27"/>
-      <c r="N54" s="54"/>
-      <c r="P54" s="17"/>
-      <c r="Q54" s="17"/>
-      <c r="R54" s="27"/>
-      <c r="S54" s="54"/>
-      <c r="T54" s="53"/>
-    </row>
-    <row r="55" spans="1:20" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="68" t="s">
+      <c r="T53" s="52"/>
+    </row>
+    <row r="54" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="25"/>
+      <c r="B54" s="25"/>
+      <c r="C54" s="25"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="25"/>
+      <c r="F54" s="25"/>
+      <c r="G54" s="25"/>
+      <c r="H54" s="25"/>
+      <c r="I54" s="25"/>
+      <c r="J54" s="16"/>
+      <c r="K54" s="16"/>
+      <c r="L54" s="25"/>
+      <c r="M54" s="26"/>
+      <c r="N54" s="53"/>
+      <c r="P54" s="16"/>
+      <c r="Q54" s="16"/>
+      <c r="R54" s="26"/>
+      <c r="S54" s="53"/>
+      <c r="T54" s="52"/>
+    </row>
+    <row r="55" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="B55" s="68"/>
-      <c r="C55" s="68"/>
-      <c r="D55" s="68"/>
-      <c r="E55" s="68"/>
-      <c r="F55" s="68"/>
-      <c r="G55" s="68"/>
-      <c r="H55" s="68"/>
-      <c r="I55" s="68"/>
-      <c r="J55" s="68"/>
-      <c r="K55" s="68"/>
-      <c r="L55" s="68"/>
-      <c r="M55" s="68"/>
-    </row>
-    <row r="56" spans="1:20" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A56" s="33" t="s">
+      <c r="B55" s="67"/>
+      <c r="C55" s="67"/>
+      <c r="D55" s="67"/>
+      <c r="E55" s="67"/>
+      <c r="F55" s="67"/>
+      <c r="G55" s="67"/>
+      <c r="H55" s="67"/>
+      <c r="I55" s="67"/>
+      <c r="J55" s="67"/>
+      <c r="K55" s="67"/>
+      <c r="L55" s="67"/>
+      <c r="M55" s="67"/>
+    </row>
+    <row r="56" spans="1:20" s="23" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A56" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B56" s="34" t="s">
+      <c r="B56" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="C56" s="34" t="s">
+      <c r="C56" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="D56" s="34" t="s">
+      <c r="D56" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="E56" s="34" t="s">
+      <c r="E56" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="F56" s="34" t="s">
+      <c r="F56" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="G56" s="34" t="s">
+      <c r="G56" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="H56" s="34" t="s">
+      <c r="H56" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="I56" s="34" t="s">
+      <c r="I56" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="J56" s="34" t="s">
+      <c r="J56" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="K56" s="34" t="s">
+      <c r="K56" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="L56" s="34" t="s">
+      <c r="L56" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="M56" s="35" t="s">
+      <c r="M56" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="N56" s="14"/>
+      <c r="N56" s="13"/>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A57" s="36">
+      <c r="A57" s="35">
         <f>4*G57*M57*E57/(300000000)</f>
         <v>700</v>
       </c>
-      <c r="B57" s="37"/>
-      <c r="C57" s="38">
+      <c r="B57" s="36"/>
+      <c r="C57" s="37">
         <f>22*LOG10(F57)+28+20*LOG10(E57/1000000000)</f>
         <v>98.258700982397926</v>
       </c>
-      <c r="D57" s="39"/>
-      <c r="E57" s="40">
+      <c r="D57" s="38"/>
+      <c r="E57" s="39">
         <v>3500000000</v>
       </c>
-      <c r="F57" s="37">
+      <c r="F57" s="36">
         <v>500</v>
       </c>
-      <c r="G57" s="37">
+      <c r="G57" s="36">
         <v>10</v>
       </c>
-      <c r="H57" s="37" t="s">
+      <c r="H57" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="I57" s="37" t="s">
+      <c r="I57" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="J57" s="37" t="s">
+      <c r="J57" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="K57" s="37" t="s">
+      <c r="K57" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="L57" s="37" t="s">
+      <c r="L57" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="M57" s="41">
-        <v>1.5</v>
-      </c>
-      <c r="N57" s="24"/>
+      <c r="M57" s="40">
+        <v>1.5</v>
+      </c>
+      <c r="N57" s="23"/>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A58" s="36">
+      <c r="A58" s="35">
         <f>4*G58*M58*E58/(300000000)</f>
         <v>700</v>
       </c>
-      <c r="B58" s="37"/>
-      <c r="C58" s="38">
+      <c r="B58" s="36"/>
+      <c r="C58" s="37">
         <f>40*LOG10(F58)+7.8-18*LOG10(G58)-18*LOG10(M58)+2*LOG10(E58/1000000000)</f>
         <v>107.71849342569828</v>
       </c>
-      <c r="D58" s="39"/>
-      <c r="E58" s="40">
+      <c r="D58" s="38"/>
+      <c r="E58" s="39">
         <v>3500000000</v>
       </c>
-      <c r="F58" s="37">
+      <c r="F58" s="36">
         <v>1000</v>
       </c>
-      <c r="G58" s="37">
+      <c r="G58" s="36">
         <v>10</v>
       </c>
-      <c r="H58" s="37" t="s">
+      <c r="H58" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="I58" s="37" t="s">
+      <c r="I58" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="J58" s="37" t="s">
+      <c r="J58" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="K58" s="37" t="s">
+      <c r="K58" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="L58" s="37" t="s">
+      <c r="L58" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="M58" s="41">
-        <v>1.5</v>
-      </c>
-      <c r="N58" s="24"/>
+      <c r="M58" s="40">
+        <v>1.5</v>
+      </c>
+      <c r="N58" s="23"/>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A59" s="36" t="s">
+      <c r="A59" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B59" s="37"/>
-      <c r="C59" s="38">
+      <c r="B59" s="36"/>
+      <c r="C59" s="37">
         <f>(36.7*LOG10(F59)+22.7+26*LOG10(E59/1000000000))</f>
         <v>135.89796831223907</v>
       </c>
-      <c r="D59" s="39"/>
-      <c r="E59" s="40">
+      <c r="D59" s="38"/>
+      <c r="E59" s="39">
         <v>3500000000</v>
       </c>
-      <c r="F59" s="37">
+      <c r="F59" s="36">
         <v>500</v>
       </c>
-      <c r="G59" s="37">
+      <c r="G59" s="36">
         <v>10</v>
       </c>
-      <c r="H59" s="37" t="s">
+      <c r="H59" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="I59" s="37" t="s">
+      <c r="I59" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="J59" s="37" t="s">
+      <c r="J59" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="K59" s="37" t="s">
+      <c r="K59" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="L59" s="37" t="s">
+      <c r="L59" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="M59" s="41">
-        <v>1.5</v>
-      </c>
-      <c r="N59" s="24"/>
+      <c r="M59" s="40">
+        <v>1.5</v>
+      </c>
+      <c r="N59" s="23"/>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A60" s="36">
+      <c r="A60" s="35">
         <f t="shared" ref="A60:A68" si="10">4*G60*M60*E60/(300000000)</f>
         <v>1750</v>
       </c>
-      <c r="B60" s="37"/>
-      <c r="C60" s="38">
+      <c r="B60" s="36"/>
+      <c r="C60" s="37">
         <f>22*LOG10(F60)+28+20*LOG10(E60/1000000000)</f>
         <v>98.258700982397926</v>
       </c>
-      <c r="D60" s="39"/>
-      <c r="E60" s="40">
+      <c r="D60" s="38"/>
+      <c r="E60" s="39">
         <v>3500000000</v>
       </c>
-      <c r="F60" s="37">
+      <c r="F60" s="36">
         <v>500</v>
       </c>
-      <c r="G60" s="37">
+      <c r="G60" s="36">
         <v>25</v>
       </c>
-      <c r="H60" s="37" t="s">
+      <c r="H60" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="I60" s="37">
-        <v>20</v>
-      </c>
-      <c r="J60" s="37">
-        <v>20</v>
-      </c>
-      <c r="K60" s="37" t="s">
+      <c r="I60" s="36">
+        <v>20</v>
+      </c>
+      <c r="J60" s="36">
+        <v>20</v>
+      </c>
+      <c r="K60" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="L60" s="37" t="s">
+      <c r="L60" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="M60" s="41">
-        <v>1.5</v>
-      </c>
-      <c r="N60" s="24"/>
+      <c r="M60" s="40">
+        <v>1.5</v>
+      </c>
+      <c r="N60" s="23"/>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A61" s="36">
+      <c r="A61" s="35">
         <f t="shared" si="10"/>
         <v>1750</v>
       </c>
-      <c r="B61" s="37"/>
-      <c r="C61" s="38">
+      <c r="B61" s="36"/>
+      <c r="C61" s="37">
         <f>40*LOG10(F61)+7.8-18*LOG10(G61)-18*LOG10(M61)+2*LOG10(E61/1000000000)</f>
         <v>112.59677309616087</v>
       </c>
-      <c r="D61" s="39"/>
-      <c r="E61" s="40">
+      <c r="D61" s="38"/>
+      <c r="E61" s="39">
         <v>3500000000</v>
       </c>
-      <c r="F61" s="37">
+      <c r="F61" s="36">
         <v>2000</v>
       </c>
-      <c r="G61" s="37">
+      <c r="G61" s="36">
         <v>25</v>
       </c>
-      <c r="H61" s="37" t="s">
+      <c r="H61" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="I61" s="37">
-        <v>20</v>
-      </c>
-      <c r="J61" s="37">
-        <v>20</v>
-      </c>
-      <c r="K61" s="37" t="s">
+      <c r="I61" s="36">
+        <v>20</v>
+      </c>
+      <c r="J61" s="36">
+        <v>20</v>
+      </c>
+      <c r="K61" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="L61" s="37" t="s">
+      <c r="L61" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="M61" s="41">
-        <v>1.5</v>
-      </c>
-      <c r="N61" s="24"/>
+      <c r="M61" s="40">
+        <v>1.5</v>
+      </c>
+      <c r="N61" s="23"/>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A62" s="36">
+      <c r="A62" s="35">
         <f t="shared" si="10"/>
         <v>1750</v>
       </c>
-      <c r="B62" s="37"/>
-      <c r="C62" s="38">
+      <c r="B62" s="36"/>
+      <c r="C62" s="37">
         <f>161.04-7.1*LOG10(J62)+7.5*LOG10(I62)-(24.37-3.7*(I62/G62)^2)*LOG10(G62)+(43.42-3.1*LOG10(G62))*(LOG10(F62)-3)+20*LOG10(E62/1000000000)-(3.2*(LOG10(11.75*M62))^2-4.97)</f>
         <v>141.68521586142342</v>
       </c>
-      <c r="D62" s="39"/>
-      <c r="E62" s="40">
+      <c r="D62" s="38"/>
+      <c r="E62" s="39">
         <v>3500000000</v>
       </c>
-      <c r="F62" s="37">
+      <c r="F62" s="36">
         <v>1000</v>
       </c>
-      <c r="G62" s="37">
+      <c r="G62" s="36">
         <v>25</v>
       </c>
-      <c r="H62" s="37" t="s">
+      <c r="H62" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="I62" s="37">
-        <v>20</v>
-      </c>
-      <c r="J62" s="37">
-        <v>20</v>
-      </c>
-      <c r="K62" s="37" t="s">
+      <c r="I62" s="36">
+        <v>20</v>
+      </c>
+      <c r="J62" s="36">
+        <v>20</v>
+      </c>
+      <c r="K62" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="L62" s="37" t="s">
+      <c r="L62" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="M62" s="41">
-        <v>1.5</v>
-      </c>
-      <c r="N62" s="24"/>
+      <c r="M62" s="40">
+        <v>1.5</v>
+      </c>
+      <c r="N62" s="23"/>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A63" s="36">
+      <c r="A63" s="35">
         <f t="shared" si="10"/>
         <v>2450</v>
       </c>
-      <c r="B63" s="39">
+      <c r="B63" s="38">
         <f>2*PI()*G63*M63*E63/(300000000)</f>
         <v>3848.4510006474966</v>
       </c>
-      <c r="C63" s="38">
+      <c r="C63" s="37">
         <f>20*LOG10(40*PI()*F63*(E63/1000000000)/3)+MIN(0.03*I63^1.72, 10)*LOG10(F63)-MIN(0.044*I63^1.72,14.77)+0.002*LOG10(I63)*F63</f>
         <v>107.73724739020315</v>
       </c>
-      <c r="D63" s="39"/>
-      <c r="E63" s="40">
+      <c r="D63" s="38"/>
+      <c r="E63" s="39">
         <v>3500000000</v>
       </c>
-      <c r="F63" s="37">
+      <c r="F63" s="36">
         <v>1000</v>
       </c>
-      <c r="G63" s="37">
+      <c r="G63" s="36">
         <v>35</v>
       </c>
-      <c r="H63" s="37" t="s">
+      <c r="H63" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="I63" s="37">
+      <c r="I63" s="36">
         <v>10</v>
       </c>
-      <c r="J63" s="37">
-        <v>20</v>
-      </c>
-      <c r="K63" s="37" t="s">
+      <c r="J63" s="36">
+        <v>20</v>
+      </c>
+      <c r="K63" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="L63" s="37" t="s">
+      <c r="L63" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="M63" s="41">
-        <v>1.5</v>
-      </c>
-      <c r="N63" s="24"/>
+      <c r="M63" s="40">
+        <v>1.5</v>
+      </c>
+      <c r="N63" s="23"/>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A64" s="36">
+      <c r="A64" s="35">
         <f t="shared" si="10"/>
         <v>2450</v>
       </c>
-      <c r="B64" s="39">
+      <c r="B64" s="38">
         <f>2*PI()*G64*M64*E64/(300000000)</f>
         <v>3848.4510006474966</v>
       </c>
-      <c r="C64" s="38">
+      <c r="C64" s="37">
         <f>(20*LOG10(40*PI()*B64*(E64/1000000000)/3)+MIN(0.03*I64^1.72, 10)*LOG10(B64)-MIN(0.044*I64^1.72,14.77)+0.002*LOG10(I64)*B64)</f>
         <v>126.06135593614999</v>
       </c>
-      <c r="D64" s="38">
+      <c r="D64" s="37">
         <f>C64+40*LOG10(F64/B64)</f>
         <v>126.73231713348109</v>
       </c>
-      <c r="E64" s="40">
+      <c r="E64" s="39">
         <v>3500000000</v>
       </c>
-      <c r="F64" s="37">
+      <c r="F64" s="36">
         <v>4000</v>
       </c>
-      <c r="G64" s="37">
+      <c r="G64" s="36">
         <v>35</v>
       </c>
-      <c r="H64" s="37" t="s">
+      <c r="H64" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="I64" s="37">
+      <c r="I64" s="36">
         <v>10</v>
       </c>
-      <c r="J64" s="37">
-        <v>20</v>
-      </c>
-      <c r="K64" s="42" t="s">
+      <c r="J64" s="36">
+        <v>20</v>
+      </c>
+      <c r="K64" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="L64" s="37" t="s">
+      <c r="L64" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="M64" s="41">
-        <v>1.5</v>
-      </c>
-      <c r="N64" s="24"/>
+      <c r="M64" s="40">
+        <v>1.5</v>
+      </c>
+      <c r="N64" s="23"/>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A65" s="36">
+      <c r="A65" s="35">
         <f t="shared" si="10"/>
         <v>2450</v>
       </c>
-      <c r="B65" s="37"/>
-      <c r="C65" s="38">
+      <c r="B65" s="36"/>
+      <c r="C65" s="37">
         <f>161.04-7.1*LOG10(J65)+7.5*LOG10(I65)-(24.37-3.7*(I65/G65)^2)*LOG10(G65)+(43.42-3.1*LOG10(G65))*(LOG10(F65)-3)+20*LOG10(E65/1000000000)-(3.2*(LOG10(11.75*M65))^2-4.97)</f>
         <v>121.39259135453526</v>
       </c>
-      <c r="D65" s="38"/>
-      <c r="E65" s="40">
+      <c r="D65" s="37"/>
+      <c r="E65" s="39">
         <v>3500000000</v>
       </c>
-      <c r="F65" s="37">
+      <c r="F65" s="36">
         <v>500</v>
       </c>
-      <c r="G65" s="37">
+      <c r="G65" s="36">
         <v>35</v>
       </c>
-      <c r="H65" s="37" t="s">
+      <c r="H65" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="I65" s="37">
+      <c r="I65" s="36">
         <v>10</v>
       </c>
-      <c r="J65" s="37">
-        <v>20</v>
-      </c>
-      <c r="K65" s="37" t="s">
+      <c r="J65" s="36">
+        <v>20</v>
+      </c>
+      <c r="K65" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="L65" s="37" t="s">
+      <c r="L65" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="M65" s="41">
-        <v>1.5</v>
-      </c>
-      <c r="N65" s="24"/>
+      <c r="M65" s="40">
+        <v>1.5</v>
+      </c>
+      <c r="N65" s="23"/>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A66" s="36">
+      <c r="A66" s="35">
         <f t="shared" si="10"/>
         <v>2450</v>
       </c>
-      <c r="B66" s="39">
+      <c r="B66" s="38">
         <f>2*PI()*G66*M66*E66/(300000000)</f>
         <v>3848.4510006474966</v>
       </c>
-      <c r="C66" s="38">
+      <c r="C66" s="37">
         <f>20*LOG10(40*PI()*F66*(E66/1000000000)/3)+MIN(0.03*I66^1.72, 10)*LOG10(F66)-MIN(0.044*I66^1.72,14.77)+0.002*LOG10(I66)*F66</f>
         <v>107.73724739020315</v>
       </c>
-      <c r="D66" s="38"/>
-      <c r="E66" s="40">
+      <c r="D66" s="37"/>
+      <c r="E66" s="39">
         <v>3500000000</v>
       </c>
-      <c r="F66" s="37">
+      <c r="F66" s="36">
         <v>1000</v>
       </c>
-      <c r="G66" s="37">
+      <c r="G66" s="36">
         <v>35</v>
       </c>
-      <c r="H66" s="37" t="s">
+      <c r="H66" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="I66" s="37">
+      <c r="I66" s="36">
         <v>10</v>
       </c>
-      <c r="J66" s="37">
-        <v>20</v>
-      </c>
-      <c r="K66" s="37" t="s">
+      <c r="J66" s="36">
+        <v>20</v>
+      </c>
+      <c r="K66" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="L66" s="37" t="s">
+      <c r="L66" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="M66" s="41">
-        <v>1.5</v>
-      </c>
-      <c r="N66" s="24"/>
+      <c r="M66" s="40">
+        <v>1.5</v>
+      </c>
+      <c r="N66" s="23"/>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A67" s="36">
+      <c r="A67" s="35">
         <f t="shared" si="10"/>
         <v>2450</v>
       </c>
-      <c r="B67" s="39">
+      <c r="B67" s="38">
         <f>2*PI()*G67*M67*E67/(300000000)</f>
         <v>3848.4510006474966</v>
       </c>
-      <c r="C67" s="38">
+      <c r="C67" s="37">
         <f>(20*LOG10(40*PI()*B67*(E67/1000000000)/3)+MIN(0.03*I67^1.72, 10)*LOG10(B67)-MIN(0.044*I67^1.72,14.77)+0.002*LOG10(I67)*B67)</f>
         <v>126.06135593614999</v>
       </c>
-      <c r="D67" s="38">
+      <c r="D67" s="37">
         <f>C67+40*LOG10(F67/B67)</f>
         <v>126.73231713348109</v>
       </c>
-      <c r="E67" s="40">
+      <c r="E67" s="39">
         <v>3500000000</v>
       </c>
-      <c r="F67" s="37">
+      <c r="F67" s="36">
         <v>4000</v>
       </c>
-      <c r="G67" s="37">
+      <c r="G67" s="36">
         <v>35</v>
       </c>
-      <c r="H67" s="37" t="s">
+      <c r="H67" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="I67" s="37">
+      <c r="I67" s="36">
         <v>10</v>
       </c>
-      <c r="J67" s="37">
-        <v>20</v>
-      </c>
-      <c r="K67" s="42" t="s">
+      <c r="J67" s="36">
+        <v>20</v>
+      </c>
+      <c r="K67" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="L67" s="37" t="s">
+      <c r="L67" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="M67" s="41">
-        <v>1.5</v>
-      </c>
-      <c r="N67" s="24"/>
+      <c r="M67" s="40">
+        <v>1.5</v>
+      </c>
+      <c r="N67" s="23"/>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A68" s="43">
+      <c r="A68" s="42">
         <f t="shared" si="10"/>
         <v>2450</v>
       </c>
-      <c r="B68" s="44"/>
-      <c r="C68" s="45">
+      <c r="B68" s="43"/>
+      <c r="C68" s="44">
         <f>161.04-7.1*LOG10(J68)+7.5*LOG10(I68)-(24.37-3.7*(I68/G68)^2)*LOG10(G68)+(43.42-3.1*LOG10(G68))*(LOG10(F68)-3)+20*LOG10(E68/1000000000)-(3.2*(LOG10(11.75*M68))^2-4.97)</f>
         <v>121.39259135453526</v>
       </c>
-      <c r="D68" s="46"/>
-      <c r="E68" s="47">
+      <c r="D68" s="45"/>
+      <c r="E68" s="46">
         <v>3500000000</v>
       </c>
-      <c r="F68" s="44">
+      <c r="F68" s="43">
         <v>500</v>
       </c>
-      <c r="G68" s="44">
+      <c r="G68" s="43">
         <v>35</v>
       </c>
-      <c r="H68" s="44" t="s">
+      <c r="H68" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="I68" s="44">
+      <c r="I68" s="43">
         <v>10</v>
       </c>
-      <c r="J68" s="44">
-        <v>20</v>
-      </c>
-      <c r="K68" s="44" t="s">
+      <c r="J68" s="43">
+        <v>20</v>
+      </c>
+      <c r="K68" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="L68" s="44" t="s">
+      <c r="L68" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="M68" s="48">
-        <v>1.5</v>
-      </c>
-      <c r="N68" s="24"/>
+      <c r="M68" s="47">
+        <v>1.5</v>
+      </c>
+      <c r="N68" s="23"/>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72">
@@ -4127,13 +4300,14 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A55:M55"/>
     <mergeCell ref="A20:N20"/>
     <mergeCell ref="A2:E2"/>
+    <mergeCell ref="N2:R2"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:E19">
-    <cfRule type="dataBar" priority="5">
+    <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4146,22 +4320,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N4:N8">
+  <conditionalFormatting sqref="K4:K18">
     <cfRule type="dataBar" priority="6">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63C384"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{817A2237-FD7A-4274-A350-00706226E78F}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K4:K18">
-    <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4175,7 +4335,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N22:N53">
-    <cfRule type="dataBar" priority="2">
+    <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4189,6 +4349,48 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57:C68">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{1D9E106F-ABDB-4C45-8973-56B92EA94E10}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S12:S18 S4:S5 S8:S9">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{4232E29B-9545-42B7-AE12-3189426569B4}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S6">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{F119C0E7-7884-4948-ACB4-B08A2294EA82}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S7">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -4197,7 +4399,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{1D9E106F-ABDB-4C45-8973-56B92EA94E10}</x14:id>
+          <x14:id>{A76E5B64-EC84-4773-B866-843530173059}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -4217,17 +4419,6 @@
             </x14:dataBar>
           </x14:cfRule>
           <xm:sqref>E4:E19</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{817A2237-FD7A-4274-A350-00706226E78F}">
-            <x14:dataBar>
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>N4:N8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{DE0E680E-9426-4D2B-B4CC-5BEF266D5F0F}">
@@ -4266,6 +4457,39 @@
           </x14:cfRule>
           <xm:sqref>C57:C68</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{4232E29B-9545-42B7-AE12-3189426569B4}">
+            <x14:dataBar>
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>S12:S18 S4:S5 S8:S9</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{F119C0E7-7884-4948-ACB4-B08A2294EA82}">
+            <x14:dataBar>
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>S6</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{A76E5B64-EC84-4773-B866-843530173059}">
+            <x14:dataBar>
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>S7</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>